<commit_message>
removed link to download pdf + update program
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9BE4C5-2281-48C2-98E3-13706DB275E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464DF2B5-7DC7-4ACA-BD29-E96EEE20F338}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="283">
   <si>
     <t xml:space="preserve">18:00 - 20:00 </t>
   </si>
@@ -1586,8 +1586,8 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1813,9 +1813,13 @@
       <c r="B12" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>260</v>
+      </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="30" t="s">
+        <v>259</v>
+      </c>
       <c r="F12" s="16" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
program including poster sessions
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464DF2B5-7DC7-4ACA-BD29-E96EEE20F338}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D783973E-6B74-4974-91B8-5A4209130FA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -770,9 +770,6 @@
     <t>closing session</t>
   </si>
   <si>
-    <t>Paulo Charruadas/ Armelle Weitz</t>
-  </si>
-  <si>
     <t>timing</t>
   </si>
   <si>
@@ -909,6 +906,9 @@
   </si>
   <si>
     <t>18:30 - …</t>
+  </si>
+  <si>
+    <t>Philippe Sosnowska</t>
   </si>
 </sst>
 </file>
@@ -1586,8 +1586,8 @@
   </sheetPr>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1606,22 +1606,22 @@
   <sheetData>
     <row r="1" spans="1:9" s="21" customFormat="1" ht="32.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="F1" s="22" t="s">
         <v>239</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1635,7 +1635,7 @@
     </row>
     <row r="3" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>0</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>2</v>
@@ -1679,16 +1679,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>215</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="26"/>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>4</v>
@@ -1715,10 +1715,10 @@
     </row>
     <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>46</v>
@@ -1739,10 +1739,10 @@
     </row>
     <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>47</v>
@@ -1762,10 +1762,10 @@
     </row>
     <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>48</v>
@@ -1785,10 +1785,10 @@
     </row>
     <row r="11" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>49</v>
@@ -1808,17 +1808,17 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>6</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>219</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>50</v>
@@ -1870,10 +1870,10 @@
     </row>
     <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>51</v>
@@ -1894,10 +1894,10 @@
     </row>
     <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>59</v>
@@ -1917,10 +1917,10 @@
     </row>
     <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>60</v>
@@ -1940,10 +1940,10 @@
     </row>
     <row r="18" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>71</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>9</v>
@@ -1981,7 +1981,7 @@
     </row>
     <row r="20" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B20" s="50" t="s">
         <v>218</v>
@@ -1999,10 +1999,10 @@
     </row>
     <row r="21" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>58</v>
@@ -2022,10 +2022,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>107</v>
@@ -2045,10 +2045,10 @@
     </row>
     <row r="23" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>108</v>
@@ -2068,10 +2068,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>127</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>170</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>169</v>
@@ -2138,16 +2138,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>16</v>
@@ -2158,7 +2158,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B28" s="51" t="s">
         <v>220</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B29" s="51" t="s">
         <v>226</v>
@@ -2192,10 +2192,10 @@
     </row>
     <row r="30" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>72</v>
@@ -2215,10 +2215,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>73</v>
@@ -2238,10 +2238,10 @@
     </row>
     <row r="32" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>74</v>
@@ -2261,10 +2261,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>75</v>
@@ -2285,7 +2285,7 @@
     </row>
     <row r="34" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B34" s="49" t="s">
         <v>17</v>
@@ -2311,7 +2311,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B36" s="50" t="s">
         <v>19</v>
@@ -2328,10 +2328,10 @@
     </row>
     <row r="37" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>78</v>
@@ -2351,10 +2351,10 @@
     </row>
     <row r="38" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>93</v>
@@ -2374,10 +2374,10 @@
     </row>
     <row r="39" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>94</v>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="40" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>95</v>
@@ -2421,10 +2421,10 @@
     </row>
     <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>96</v>
@@ -2445,10 +2445,10 @@
     </row>
     <row r="42" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>97</v>
@@ -2468,10 +2468,10 @@
     </row>
     <row r="43" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>98</v>
@@ -2491,10 +2491,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>99</v>
@@ -2514,17 +2514,17 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D45" s="10"/>
       <c r="E45" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F45" s="16" t="s">
         <v>21</v>
@@ -2535,7 +2535,7 @@
     </row>
     <row r="46" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B46" s="50" t="s">
         <v>219</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="47" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B47" s="50" t="s">
         <v>228</v>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>101</v>
@@ -2592,18 +2592,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C49" s="12" t="s">
         <v>110</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>236</v>
+        <v>282</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>109</v>
@@ -2617,10 +2617,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>111</v>
@@ -2641,10 +2641,10 @@
     </row>
     <row r="51" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C51" s="12" t="s">
         <v>112</v>
@@ -2664,10 +2664,10 @@
     </row>
     <row r="52" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>113</v>
@@ -2687,10 +2687,10 @@
     </row>
     <row r="53" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>114</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B54" s="50" t="s">
         <v>9</v>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B55" s="50" t="s">
         <v>23</v>
@@ -2745,10 +2745,10 @@
     </row>
     <row r="56" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C56" s="12" t="s">
         <v>125</v>
@@ -2768,10 +2768,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C57" s="12" t="s">
         <v>128</v>
@@ -2791,10 +2791,10 @@
     </row>
     <row r="58" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>134</v>
@@ -2815,10 +2815,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>135</v>
@@ -2838,10 +2838,10 @@
     </row>
     <row r="60" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>136</v>
@@ -2861,10 +2861,10 @@
     </row>
     <row r="61" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C61" s="12" t="s">
         <v>137</v>
@@ -2884,7 +2884,7 @@
     </row>
     <row r="62" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B62" s="49" t="s">
         <v>26</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B64" s="50" t="s">
         <v>19</v>
@@ -2927,10 +2927,10 @@
     </row>
     <row r="65" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>143</v>
@@ -2950,10 +2950,10 @@
     </row>
     <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>144</v>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="67" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C67" s="12" t="s">
         <v>145</v>
@@ -2996,10 +2996,10 @@
     </row>
     <row r="68" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>146</v>
@@ -3019,10 +3019,10 @@
     </row>
     <row r="69" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C69" s="12" t="s">
         <v>147</v>
@@ -3042,10 +3042,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>148</v>
@@ -3065,10 +3065,10 @@
     </row>
     <row r="71" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>149</v>
@@ -3088,10 +3088,10 @@
     </row>
     <row r="72" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>171</v>
@@ -3100,7 +3100,7 @@
         <v>172</v>
       </c>
       <c r="E72" s="11" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F72" s="16" t="s">
         <v>27</v>
@@ -3111,16 +3111,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F73" s="16" t="s">
         <v>28</v>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="74" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B74" s="50" t="s">
         <v>219</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B75" s="53" t="s">
         <v>228</v>
@@ -3165,10 +3165,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>173</v>
@@ -3188,10 +3188,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>175</v>
@@ -3211,10 +3211,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>176</v>
@@ -3234,10 +3234,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>177</v>
@@ -3257,10 +3257,10 @@
     </row>
     <row r="80" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>178</v>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>179</v>
@@ -3303,7 +3303,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B82" s="50" t="s">
         <v>9</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B83" s="50" t="s">
         <v>218</v>
@@ -3337,10 +3337,10 @@
     </row>
     <row r="84" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>180</v>
@@ -3360,10 +3360,10 @@
     </row>
     <row r="85" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>181</v>
@@ -3383,10 +3383,10 @@
     </row>
     <row r="86" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C86" s="12" t="s">
         <v>202</v>
@@ -3406,10 +3406,10 @@
     </row>
     <row r="87" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C87" s="12" t="s">
         <v>203</v>
@@ -3429,10 +3429,10 @@
     </row>
     <row r="88" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>204</v>
@@ -3452,10 +3452,10 @@
     </row>
     <row r="89" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>174</v>
@@ -3475,16 +3475,16 @@
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F90" s="16" t="s">
         <v>31</v>
@@ -3495,7 +3495,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B91" s="51" t="s">
         <v>220</v>
@@ -3512,7 +3512,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B92" s="50" t="s">
         <v>233</v>
@@ -3529,10 +3529,10 @@
     </row>
     <row r="93" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C93" s="12" t="s">
         <v>210</v>
@@ -3552,10 +3552,10 @@
     </row>
     <row r="94" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>213</v>
@@ -3575,7 +3575,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B95" s="50" t="s">
         <v>234</v>
@@ -3592,16 +3592,16 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C96" s="55" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="10"/>
@@ -3611,10 +3611,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C97" s="55" t="s">
         <v>32</v>
@@ -3628,10 +3628,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B98" s="49" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C98" s="42" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
updated program + chairs
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B46446-973D-4025-B276-1A0CB0E0F1AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407FF050-B8A1-484D-801C-E951B6B91C5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="program with all time slots" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk65507359" localSheetId="0">'ORAL and POSTER PRESENTATIONS'!$D$65</definedName>
+    <definedName name="_Hlk65507359" localSheetId="0">'ORAL and POSTER PRESENTATIONS'!$D$72</definedName>
     <definedName name="_Hlk65507359" localSheetId="1">'program with all time slots'!$D$65</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="386">
   <si>
     <t>day</t>
   </si>
@@ -1147,9 +1147,6 @@
     <t>session 1</t>
   </si>
   <si>
-    <t xml:space="preserve">chair: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Advancing Elm dendrochronology in the United Kingdom </t>
   </si>
   <si>
@@ -1172,13 +1169,76 @@
   </si>
   <si>
     <t>The Rosewoods, where fine arts and nature conservation meet: the importance of identifying wood to the species level and the methods to do that</t>
+  </si>
+  <si>
+    <t>Built heritage</t>
+  </si>
+  <si>
+    <t>chair:</t>
+  </si>
+  <si>
+    <t>Shipwrecks and archaeological structures</t>
+  </si>
+  <si>
+    <t>Furniture and works of art</t>
+  </si>
+  <si>
+    <t>Forest history</t>
+  </si>
+  <si>
+    <t>session 5</t>
+  </si>
+  <si>
+    <t>Evidence of timber trade and transport</t>
+  </si>
+  <si>
+    <t>Novel methods for dating and provenance analysis</t>
+  </si>
+  <si>
+    <t>Non-invasive techniques for the study of wooden cultural heritage</t>
+  </si>
+  <si>
+    <t>(chair: Gabri van Tussenbroek)</t>
+  </si>
+  <si>
+    <t>(chair: Mike Belasus)</t>
+  </si>
+  <si>
+    <t>(chair: Paul van Duin)</t>
+  </si>
+  <si>
+    <t>12:30 - 12:45</t>
+  </si>
+  <si>
+    <t>12:45 - 13:45</t>
+  </si>
+  <si>
+    <t>(chair: tba)</t>
+  </si>
+  <si>
+    <t>(chair: Neil Loader)</t>
+  </si>
+  <si>
+    <t>(chair: Francien Bossema)</t>
+  </si>
+  <si>
+    <t>poster</t>
+  </si>
+  <si>
+    <t>(chair: Anne Crone)</t>
+  </si>
+  <si>
+    <t>(chair: Roberta D'Andrea)</t>
+  </si>
+  <si>
+    <t>S5-O-014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1296,6 +1356,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1378,7 +1452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1553,6 +1627,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1872,10 +1958,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95:G124"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89:G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1975,7 +2061,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>15</v>
@@ -1998,33 +2084,25 @@
         <v>356</v>
       </c>
       <c r="D7" s="48"/>
-      <c r="E7" s="49" t="s">
-        <v>357</v>
+      <c r="E7" s="30" t="s">
+        <v>365</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>341</v>
-      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="30" t="s">
+        <v>374</v>
+      </c>
+      <c r="F8" s="27"/>
       <c r="G8" s="1">
         <v>4</v>
       </c>
@@ -2033,17 +2111,17 @@
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>23</v>
+      <c r="B9" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>341</v>
@@ -2057,16 +2135,16 @@
         <v>11</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>341</v>
@@ -2075,21 +2153,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>341</v>
@@ -2102,97 +2180,99 @@
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="48"/>
+      <c r="B12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>341</v>
+      </c>
       <c r="G12" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="45"/>
-      <c r="C13" s="47" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="26" t="s">
+      <c r="B13" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>341</v>
       </c>
       <c r="G13" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>341</v>
-      </c>
+      <c r="B14" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="48"/>
       <c r="G14" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>341</v>
-      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="30" t="s">
+        <v>365</v>
+      </c>
+      <c r="F15" s="27"/>
       <c r="G15" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="45"/>
+      <c r="B16" s="45" t="s">
+        <v>382</v>
+      </c>
       <c r="C16" s="47" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F16" s="26" t="s">
         <v>341</v>
@@ -2205,15 +2285,17 @@
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="45"/>
+      <c r="B17" s="45" t="s">
+        <v>382</v>
+      </c>
       <c r="C17" s="47" t="s">
-        <v>344</v>
+        <v>264</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F17" s="26" t="s">
         <v>341</v>
@@ -2226,15 +2308,17 @@
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="45"/>
+      <c r="B18" s="45" t="s">
+        <v>382</v>
+      </c>
       <c r="C18" s="47" t="s">
-        <v>345</v>
+        <v>267</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F18" s="26" t="s">
         <v>341</v>
@@ -2243,36 +2327,48 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="27"/>
+      <c r="B19" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>341</v>
+      </c>
       <c r="G19" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49" t="s">
-        <v>357</v>
-      </c>
-      <c r="F20" s="27"/>
+      <c r="B20" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>341</v>
+      </c>
       <c r="G20" s="1">
         <v>16</v>
       </c>
@@ -2281,110 +2377,90 @@
       <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="B21" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="26" t="s">
         <v>341</v>
       </c>
       <c r="G21" s="1">
         <v>17</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="B22" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="27"/>
       <c r="G22" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48" t="s">
+        <v>367</v>
+      </c>
+      <c r="F23" s="27"/>
       <c r="G23" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="B24" s="40"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="61" t="s">
+        <v>375</v>
+      </c>
+      <c r="F24" s="60"/>
       <c r="G24" s="1">
         <v>20</v>
       </c>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="18" t="s">
-        <v>68</v>
+      <c r="B25" s="44" t="s">
+        <v>52</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>59</v>
@@ -2392,23 +2468,22 @@
       <c r="G25" s="1">
         <v>21</v>
       </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>59</v>
@@ -2416,107 +2491,115 @@
       <c r="G26" s="1">
         <v>22</v>
       </c>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="27"/>
+      <c r="B27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="G27" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="27"/>
+      <c r="B28" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="G28" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="G29" s="1">
         <v>25</v>
       </c>
+      <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>88</v>
+        <v>73</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>343</v>
+        <v>59</v>
       </c>
       <c r="G30" s="1">
         <v>26</v>
       </c>
+      <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>85</v>
-      </c>
+      <c r="B31" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="38"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="27"/>
       <c r="G31" s="1">
         <v>27</v>
       </c>
@@ -2525,1509 +2608,1505 @@
       <c r="A32" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>343</v>
-      </c>
+      <c r="B32" s="40"/>
+      <c r="C32" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="27"/>
       <c r="G32" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>99</v>
+        <v>81</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="G33" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>105</v>
+        <v>207</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>107</v>
+        <v>343</v>
       </c>
       <c r="G34" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="48"/>
+      <c r="B35" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>85</v>
+      </c>
       <c r="G35" s="1">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="45"/>
-      <c r="C36" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="E36" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="F36" s="26" t="s">
-        <v>59</v>
+      <c r="B36" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>343</v>
       </c>
       <c r="G36" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="45"/>
-      <c r="C37" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E37" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>59</v>
+      <c r="B37" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="G37" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>59</v>
+      <c r="B38" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>107</v>
       </c>
       <c r="G38" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>59</v>
-      </c>
+      <c r="B39" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="41"/>
+      <c r="E39" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F39" s="48"/>
       <c r="G39" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>59</v>
-      </c>
+      <c r="B40" s="40"/>
+      <c r="C40" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" s="41"/>
+      <c r="E40" s="62" t="s">
+        <v>367</v>
+      </c>
+      <c r="F40" s="48"/>
       <c r="G40" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C41" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="38"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="27"/>
+      <c r="B41" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>59</v>
+      </c>
       <c r="G41" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="38"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="27"/>
+      <c r="B42" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>59</v>
+      </c>
       <c r="G42" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" s="15" t="s">
+      <c r="B43" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F43" s="26" t="s">
         <v>59</v>
       </c>
       <c r="G43" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="F44" s="15" t="s">
+      <c r="B44" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="26" t="s">
         <v>59</v>
       </c>
       <c r="G44" s="1">
         <v>40</v>
       </c>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" s="15" t="s">
+      <c r="B45" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" s="26" t="s">
         <v>59</v>
       </c>
       <c r="G45" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F46" s="48"/>
+      <c r="B46" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="38"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="27"/>
       <c r="G46" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="17" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="46"/>
+      <c r="C47" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" s="38"/>
+      <c r="E47" s="62" t="s">
+        <v>367</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G49" s="1">
+        <v>45</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F50" s="48"/>
+      <c r="G50" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="24"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="48" t="s">
-        <v>347</v>
-      </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="49" t="s">
-        <v>357</v>
-      </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="G49" s="1">
-        <v>2</v>
-      </c>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="G50" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="G51" s="1">
-        <v>4</v>
-      </c>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C51" s="12"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="24"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>149</v>
-      </c>
+      <c r="B52" s="40"/>
+      <c r="C52" s="48" t="s">
+        <v>347</v>
+      </c>
+      <c r="D52" s="27"/>
+      <c r="E52" s="62" t="s">
+        <v>368</v>
+      </c>
+      <c r="F52" s="27"/>
       <c r="G52" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>149</v>
-      </c>
+      <c r="B53" s="40"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="62" t="s">
+        <v>376</v>
+      </c>
+      <c r="F53" s="27"/>
       <c r="G53" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G54" s="1">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G55" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>31</v>
+        <v>154</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F56" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G56" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B57" s="40" t="s">
-        <v>174</v>
-      </c>
-      <c r="C57" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="D57" s="48"/>
-      <c r="E57" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="48"/>
+      <c r="B57" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>149</v>
+      </c>
       <c r="G57" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B58" s="45"/>
-      <c r="C58" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="D58" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="E58" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="F58" s="26" t="s">
+      <c r="B58" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F58" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G58" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B59" s="45"/>
-      <c r="C59" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="D59" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="E59" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="F59" s="26" t="s">
+      <c r="B59" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F59" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G59" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="45"/>
-      <c r="C60" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="D60" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="E60" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="F60" s="26" t="s">
+      <c r="B60" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F60" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G60" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B61" s="45"/>
-      <c r="C61" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="E61" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="F61" s="26" t="s">
+      <c r="B61" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F61" s="15" t="s">
         <v>149</v>
       </c>
       <c r="G61" s="1">
-        <v>14</v>
-      </c>
-      <c r="I61" s="3"/>
-    </row>
-    <row r="62" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B62" s="45"/>
-      <c r="C62" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="D62" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="E62" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="F62" s="26" t="s">
-        <v>149</v>
-      </c>
+      <c r="B62" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C62" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" s="48"/>
+      <c r="E62" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F62" s="48"/>
       <c r="G62" s="1">
-        <v>15</v>
-      </c>
-      <c r="I62" s="3"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B63" s="40" t="s">
-        <v>190</v>
-      </c>
-      <c r="C63" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="D63" s="41"/>
-      <c r="E63" s="30"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="48" t="s">
+        <v>347</v>
+      </c>
+      <c r="D63" s="27"/>
+      <c r="E63" s="62" t="s">
+        <v>368</v>
+      </c>
       <c r="F63" s="27"/>
       <c r="G63" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B64" s="40"/>
-      <c r="C64" s="41" t="s">
-        <v>348</v>
-      </c>
-      <c r="D64" s="41"/>
-      <c r="E64" s="49" t="s">
-        <v>357</v>
-      </c>
-      <c r="F64" s="27"/>
+      <c r="B64" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D64" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="F64" s="26" t="s">
+        <v>149</v>
+      </c>
       <c r="G64" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B65" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>342</v>
+      <c r="B65" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="G65" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B66" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="F66" s="15" t="s">
-        <v>342</v>
+      <c r="B66" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="F66" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="G66" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B67" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="F67" s="15" t="s">
-        <v>342</v>
+      <c r="B67" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="G67" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B68" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="F68" s="15" t="s">
-        <v>342</v>
+      <c r="B68" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="D68" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="G68" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B69" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>342</v>
-      </c>
+      <c r="B69" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D69" s="41"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="27"/>
       <c r="G69" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F70" s="15" t="s">
-        <v>342</v>
-      </c>
+      <c r="B70" s="40"/>
+      <c r="C70" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="D70" s="41"/>
+      <c r="E70" s="62" t="s">
+        <v>369</v>
+      </c>
+      <c r="F70" s="27"/>
       <c r="G70" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B71" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C71" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D71" s="51"/>
-      <c r="E71" s="32"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="41"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="62" t="s">
+        <v>384</v>
+      </c>
       <c r="F71" s="27"/>
       <c r="G71" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B72" s="40"/>
-      <c r="C72" s="48" t="s">
-        <v>211</v>
-      </c>
-      <c r="D72" s="32"/>
-      <c r="E72" s="49" t="s">
-        <v>357</v>
-      </c>
-      <c r="F72" s="27"/>
+      <c r="B72" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>342</v>
+      </c>
       <c r="G72" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>346</v>
+        <v>87</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>214</v>
+        <v>196</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>342</v>
       </c>
       <c r="G73" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D74" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="E74" s="10" t="s">
-        <v>217</v>
+        <v>20</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E74" s="8" t="s">
+        <v>200</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>218</v>
+        <v>342</v>
       </c>
       <c r="G74" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="D75" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>221</v>
+        <v>24</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>203</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>218</v>
+        <v>342</v>
       </c>
       <c r="G75" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>223</v>
+        <v>28</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="F76" s="15" t="s">
-        <v>218</v>
+        <v>342</v>
       </c>
       <c r="G76" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="E77" s="10" t="s">
-        <v>227</v>
+        <v>32</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>209</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>218</v>
+        <v>342</v>
       </c>
       <c r="G77" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>103</v>
+        <v>377</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>230</v>
+        <v>346</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>214</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>218</v>
+        <v>342</v>
       </c>
       <c r="G78" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
         <v>143</v>
       </c>
       <c r="B79" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="C79" s="48"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="48" t="s">
-        <v>232</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D79" s="51"/>
+      <c r="E79" s="32"/>
       <c r="F79" s="27"/>
       <c r="G79" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="C80" s="14"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="24"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" s="40"/>
+      <c r="C80" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="D80" s="41"/>
+      <c r="E80" s="62" t="s">
+        <v>371</v>
+      </c>
+      <c r="F80" s="27"/>
+      <c r="G80" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B81" s="40"/>
-      <c r="C81" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="D81" s="43"/>
-      <c r="E81" s="49" t="s">
-        <v>357</v>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="62" t="s">
+        <v>383</v>
       </c>
       <c r="F81" s="27"/>
       <c r="G81" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>145</v>
+        <v>86</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="F82" s="15" t="s">
         <v>218</v>
       </c>
       <c r="G82" s="1">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="F83" s="15" t="s">
         <v>218</v>
       </c>
       <c r="G83" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="F84" s="15" t="s">
         <v>218</v>
       </c>
       <c r="G84" s="1">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="F85" s="15" t="s">
         <v>218</v>
       </c>
       <c r="G85" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
-        <v>234</v>
+        <v>143</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="F86" s="15" t="s">
         <v>218</v>
       </c>
       <c r="G86" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="34.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B87" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C87" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="F87" s="15" t="s">
-        <v>218</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="B87" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="C87" s="48"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="F87" s="27"/>
       <c r="G87" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A88" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="F88" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="G88" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C88" s="14"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="24"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B89" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="F89" s="15" t="s">
-        <v>260</v>
-      </c>
+      <c r="B89" s="40"/>
+      <c r="C89" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="D89" s="41"/>
+      <c r="E89" s="62" t="s">
+        <v>371</v>
+      </c>
+      <c r="F89" s="27"/>
       <c r="G89" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B90" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C90" s="55" t="s">
-        <v>36</v>
-      </c>
+      <c r="B90" s="40"/>
+      <c r="C90" s="41"/>
       <c r="D90" s="41"/>
-      <c r="E90" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F90" s="48"/>
+      <c r="E90" s="62" t="s">
+        <v>379</v>
+      </c>
+      <c r="F90" s="27"/>
       <c r="G90" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A91" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C91" s="54" t="s">
-        <v>359</v>
-      </c>
-      <c r="D91" s="31" t="s">
-        <v>265</v>
-      </c>
-      <c r="E91" s="31" t="s">
-        <v>266</v>
-      </c>
-      <c r="F91" s="26" t="s">
-        <v>342</v>
+      <c r="B91" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F91" s="15" t="s">
+        <v>218</v>
       </c>
       <c r="G91" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C92" s="54" t="s">
-        <v>360</v>
-      </c>
-      <c r="D92" s="31" t="s">
-        <v>268</v>
-      </c>
-      <c r="E92" s="31" t="s">
-        <v>269</v>
-      </c>
-      <c r="F92" s="26" t="s">
-        <v>342</v>
+      <c r="B92" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>218</v>
       </c>
       <c r="G92" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A93" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C93" s="54" t="s">
-        <v>361</v>
-      </c>
-      <c r="D93" s="31" t="s">
-        <v>362</v>
-      </c>
-      <c r="E93" s="31" t="s">
-        <v>272</v>
-      </c>
-      <c r="F93" s="26" t="s">
-        <v>342</v>
+      <c r="B93" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>218</v>
       </c>
       <c r="G93" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="C94" s="47" t="s">
-        <v>312</v>
-      </c>
-      <c r="D94" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="E94" s="31" t="s">
-        <v>313</v>
-      </c>
-      <c r="F94" s="26" t="s">
+      <c r="B94" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F94" s="15" t="s">
         <v>218</v>
       </c>
       <c r="G94" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B95" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C95" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="D95" s="38"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="43"/>
+      <c r="B95" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>218</v>
+      </c>
       <c r="G95" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B96" s="52"/>
-      <c r="C96" s="53" t="s">
-        <v>273</v>
-      </c>
-      <c r="D96" s="41"/>
-      <c r="E96" s="49" t="s">
-        <v>357</v>
-      </c>
-      <c r="F96" s="43"/>
+      <c r="B96" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>218</v>
+      </c>
       <c r="G96" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A97" s="9" t="s">
         <v>234</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>274</v>
+        <v>27</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>254</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>358</v>
+        <v>256</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>260</v>
+        <v>218</v>
       </c>
       <c r="G97" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A98" s="9" t="s">
         <v>234</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>277</v>
+        <v>31</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>385</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="F98" s="15" t="s">
         <v>260</v>
       </c>
       <c r="G98" s="1">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B99" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="E99" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="F99" s="15" t="s">
-        <v>260</v>
-      </c>
+      <c r="B99" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C99" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D99" s="41"/>
+      <c r="E99" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F99" s="48"/>
       <c r="G99" s="1">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B100" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="E100" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="F100" s="15" t="s">
-        <v>260</v>
-      </c>
+      <c r="B100" s="40"/>
+      <c r="C100" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="D100" s="41"/>
+      <c r="E100" s="62" t="s">
+        <v>369</v>
+      </c>
+      <c r="F100" s="27"/>
       <c r="G100" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B101" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="E101" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="F101" s="15" t="s">
-        <v>260</v>
+      <c r="B101" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="C101" s="54" t="s">
+        <v>358</v>
+      </c>
+      <c r="D101" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="E101" s="31" t="s">
+        <v>266</v>
+      </c>
+      <c r="F101" s="26" t="s">
+        <v>342</v>
       </c>
       <c r="G101" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A102" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B102" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="D102" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="E102" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="F102" s="15" t="s">
-        <v>260</v>
+      <c r="B102" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="C102" s="54" t="s">
+        <v>359</v>
+      </c>
+      <c r="D102" s="31" t="s">
+        <v>268</v>
+      </c>
+      <c r="E102" s="31" t="s">
+        <v>269</v>
+      </c>
+      <c r="F102" s="26" t="s">
+        <v>342</v>
       </c>
       <c r="G102" s="1">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B103" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C103" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="D103" s="51"/>
-      <c r="E103" s="32"/>
-      <c r="F103" s="27"/>
+      <c r="B103" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="C103" s="54" t="s">
+        <v>360</v>
+      </c>
+      <c r="D103" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="E103" s="31" t="s">
+        <v>272</v>
+      </c>
+      <c r="F103" s="26" t="s">
+        <v>342</v>
+      </c>
       <c r="G103" s="1">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -4035,437 +4114,761 @@
         <v>234</v>
       </c>
       <c r="B104" s="40"/>
-      <c r="C104" s="48" t="s">
-        <v>292</v>
-      </c>
-      <c r="D104" s="50"/>
-      <c r="E104" s="49" t="s">
-        <v>357</v>
+      <c r="C104" s="41" t="s">
+        <v>370</v>
+      </c>
+      <c r="D104" s="41"/>
+      <c r="E104" s="62" t="s">
+        <v>371</v>
       </c>
       <c r="F104" s="27"/>
       <c r="G104" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A105" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B105" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="D105" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="E105" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="F105" s="15" t="s">
+      <c r="B105" s="63" t="s">
+        <v>382</v>
+      </c>
+      <c r="C105" s="47" t="s">
+        <v>312</v>
+      </c>
+      <c r="D105" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="F105" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="G105" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B106" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C106" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D106" s="38"/>
+      <c r="E106" s="30"/>
+      <c r="F106" s="43"/>
+      <c r="G106" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B107" s="40"/>
+      <c r="C107" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="D107" s="41"/>
+      <c r="E107" s="62" t="s">
+        <v>372</v>
+      </c>
+      <c r="F107" s="27"/>
+      <c r="G107" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B108" s="40"/>
+      <c r="C108" s="41" t="s">
+        <v>366</v>
+      </c>
+      <c r="D108" s="41"/>
+      <c r="E108" s="62" t="s">
+        <v>380</v>
+      </c>
+      <c r="F108" s="27"/>
+      <c r="G108" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B109" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="E109" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="F109" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G105" s="1">
+      <c r="G109" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B110" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="D110" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G110" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G111" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="F112" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G112" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A113" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B113" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G113" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A106" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B106" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="E106" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="F106" s="15" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B114" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F114" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G106" s="1">
+      <c r="G114" s="1">
         <v>26</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A107" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B107" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="D107" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="E107" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F107" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="G107" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A108" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B108" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="D108" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="E108" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="F108" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="G108" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B109" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="D109" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="E109" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="F109" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="G109" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B110" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>309</v>
-      </c>
-      <c r="D110" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="E110" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="F110" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="G110" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B111" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="C111" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D111" s="41"/>
-      <c r="E111" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="F111" s="48"/>
-      <c r="G111" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B112" s="45"/>
-      <c r="C112" s="47" t="s">
-        <v>363</v>
-      </c>
-      <c r="D112" s="31" t="s">
-        <v>364</v>
-      </c>
-      <c r="E112" s="31" t="s">
-        <v>365</v>
-      </c>
-      <c r="F112" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="G112" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B113" s="45"/>
-      <c r="C113" s="47" t="s">
-        <v>314</v>
-      </c>
-      <c r="D113" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="E113" s="31" t="s">
-        <v>315</v>
-      </c>
-      <c r="F113" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="G113" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B114" s="45"/>
-      <c r="C114" s="47" t="s">
-        <v>316</v>
-      </c>
-      <c r="D114" s="31" t="s">
-        <v>317</v>
-      </c>
-      <c r="E114" s="31" t="s">
-        <v>318</v>
-      </c>
-      <c r="F114" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="G114" s="1">
-        <v>34</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B115" s="45"/>
-      <c r="C115" s="47" t="s">
-        <v>319</v>
-      </c>
-      <c r="D115" s="31" t="s">
-        <v>320</v>
-      </c>
-      <c r="E115" s="31" t="s">
-        <v>321</v>
-      </c>
-      <c r="F115" s="26" t="s">
-        <v>302</v>
-      </c>
+      <c r="B115" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C115" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D115" s="51"/>
+      <c r="E115" s="32"/>
+      <c r="F115" s="27"/>
       <c r="G115" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B116" s="45"/>
-      <c r="C116" s="47" t="s">
-        <v>322</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>323</v>
-      </c>
-      <c r="E116" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="F116" s="26" t="s">
-        <v>302</v>
-      </c>
+      <c r="B116" s="40"/>
+      <c r="C116" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="D116" s="41"/>
+      <c r="E116" s="62" t="s">
+        <v>372</v>
+      </c>
+      <c r="F116" s="27"/>
       <c r="G116" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A117" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B117" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C117" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="D117" s="38"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="27"/>
+      <c r="B117" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D117" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="E117" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="F117" s="15" t="s">
+        <v>260</v>
+      </c>
       <c r="G117" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A118" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B118" s="40"/>
-      <c r="C118" s="48" t="s">
+      <c r="B118" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D118" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="F118" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G118" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" s="40"/>
+      <c r="C119" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="D118" s="50"/>
-      <c r="E118" s="50"/>
-      <c r="F118" s="27"/>
-      <c r="G118" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A119" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B119" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="C119" s="11" t="s">
-        <v>327</v>
-      </c>
-      <c r="D119" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="E119" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="F119" s="15" t="s">
-        <v>302</v>
-      </c>
+      <c r="D119" s="41"/>
+      <c r="E119" s="62" t="s">
+        <v>373</v>
+      </c>
+      <c r="F119" s="27"/>
       <c r="G119" s="1">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="40"/>
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
+      <c r="E120" s="62" t="s">
+        <v>381</v>
+      </c>
+      <c r="F120" s="27"/>
+      <c r="G120" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A121" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B121" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D121" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F121" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G121" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A122" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B122" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="D122" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="E122" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="F122" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G122" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B123" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="F123" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G123" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B124" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="D124" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="F124" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G124" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B125" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C125" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D125" s="41"/>
+      <c r="E125" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F125" s="48"/>
+      <c r="G125" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B126" s="40"/>
+      <c r="C126" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="D126" s="41"/>
+      <c r="E126" s="62" t="s">
+        <v>372</v>
+      </c>
+      <c r="F126" s="27"/>
+      <c r="G126" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B127" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C127" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="D127" s="31" t="s">
+        <v>363</v>
+      </c>
+      <c r="E127" s="31" t="s">
+        <v>364</v>
+      </c>
+      <c r="F127" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G127" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B128" s="40"/>
+      <c r="C128" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="D128" s="41"/>
+      <c r="E128" s="62" t="s">
+        <v>373</v>
+      </c>
+      <c r="F128" s="27"/>
+      <c r="G128" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B129" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C129" s="47" t="s">
+        <v>314</v>
+      </c>
+      <c r="D129" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="E129" s="31" t="s">
+        <v>315</v>
+      </c>
+      <c r="F129" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G129" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B130" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C130" s="47" t="s">
+        <v>316</v>
+      </c>
+      <c r="D130" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="E130" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="F130" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G130" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B131" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C131" s="47" t="s">
+        <v>319</v>
+      </c>
+      <c r="D131" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="E131" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="F131" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G131" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B132" s="45" t="s">
+        <v>382</v>
+      </c>
+      <c r="C132" s="47" t="s">
+        <v>322</v>
+      </c>
+      <c r="D132" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="E132" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="F132" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="G132" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B133" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C133" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D133" s="38"/>
+      <c r="E133" s="30"/>
+      <c r="F133" s="27"/>
+      <c r="G133" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B134" s="40"/>
+      <c r="C134" s="41" t="s">
+        <v>326</v>
+      </c>
+      <c r="D134" s="41"/>
+      <c r="E134" s="62" t="s">
+        <v>373</v>
+      </c>
+      <c r="F134" s="27"/>
+      <c r="G134" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A135" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B135" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="C135" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="D135" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="E135" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="F135" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G135" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B136" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C136" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="D120" s="10" t="s">
+      <c r="D136" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="E120" s="10" t="s">
+      <c r="E136" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="F120" s="15" t="s">
+      <c r="F136" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G120" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B121" s="40"/>
-      <c r="C121" s="48" t="s">
+      <c r="G136" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B137" s="40"/>
+      <c r="C137" s="48" t="s">
         <v>334</v>
       </c>
-      <c r="D121" s="50"/>
-      <c r="E121" s="50"/>
-      <c r="F121" s="27"/>
-      <c r="G121" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A122" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B122" s="18" t="s">
+      <c r="D137" s="50"/>
+      <c r="E137" s="50"/>
+      <c r="F137" s="27"/>
+      <c r="G137" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B138" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="C122" s="42" t="s">
+      <c r="C138" s="42" t="s">
         <v>336</v>
       </c>
-      <c r="D122" s="9" t="s">
+      <c r="D138" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E122" s="7"/>
-      <c r="F122" s="9"/>
-      <c r="G122" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A123" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B123" s="18" t="s">
+      <c r="E138" s="7"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B139" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="C123" s="42" t="s">
+      <c r="C139" s="42" t="s">
         <v>338</v>
       </c>
-      <c r="D123" s="9"/>
-      <c r="E123" s="35"/>
-      <c r="F123" s="15"/>
-      <c r="G123" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="B124" s="40" t="s">
+      <c r="D139" s="9"/>
+      <c r="E139" s="35"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B140" s="40" t="s">
         <v>339</v>
       </c>
-      <c r="C124" s="38"/>
-      <c r="D124" s="30"/>
-      <c r="E124" s="41" t="s">
+      <c r="C140" s="38"/>
+      <c r="D140" s="30"/>
+      <c r="E140" s="41" t="s">
         <v>340</v>
       </c>
-      <c r="F124" s="27"/>
-      <c r="G124" s="1">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B131" s="18"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B132" s="18"/>
+      <c r="F140" s="27"/>
+      <c r="G140" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" s="18"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
tentativ program 3 (chair update)
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B012AF-4091-40FE-844C-B09B95B347F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9FDB9-43E9-44A4-B977-43BB1C10D718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="374">
   <si>
     <t>day</t>
   </si>
@@ -1176,6 +1176,9 @@
   </si>
   <si>
     <t>Closing session</t>
+  </si>
+  <si>
+    <t>(chair: tba)</t>
   </si>
 </sst>
 </file>
@@ -1951,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3808,7 +3811,7 @@
       <c r="C90" s="30"/>
       <c r="D90" s="26"/>
       <c r="E90" s="36" t="s">
-        <v>216</v>
+        <v>373</v>
       </c>
       <c r="F90" s="30"/>
       <c r="G90" s="6">
@@ -4205,7 +4208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>236</v>
       </c>

</xml_diff>

<commit_message>
update program - adding Brita and cancellations
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9FDB9-43E9-44A4-B977-43BB1C10D718}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2406731-CE75-4E45-B096-82F77DEB8AB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="374">
   <si>
     <t>day</t>
   </si>
@@ -848,15 +848,6 @@
     <t>S4-P-002</t>
   </si>
   <si>
-    <t>Sveva Longo</t>
-  </si>
-  <si>
-    <t>Dendrochronological investigation of monumental trees from “Villa Medicea di Castello” in Florence, Italy</t>
-  </si>
-  <si>
-    <t>S4-P-003</t>
-  </si>
-  <si>
     <t>S5-P-001</t>
   </si>
   <si>
@@ -1019,9 +1010,6 @@
     <t>Old Wood in a New Light – A dendrochronological database</t>
   </si>
   <si>
-    <t>Discussion</t>
-  </si>
-  <si>
     <t>DINNER &amp; PARTY</t>
   </si>
   <si>
@@ -1046,12 +1034,6 @@
     <t>15:00 - 15:30</t>
   </si>
   <si>
-    <t>16:15 - 16:45</t>
-  </si>
-  <si>
-    <t>16:45 - 17:00</t>
-  </si>
-  <si>
     <t>Clossing words</t>
   </si>
   <si>
@@ -1179,13 +1161,31 @@
   </si>
   <si>
     <t>(chair: tba)</t>
+  </si>
+  <si>
+    <t>Brita Lorentzen</t>
+  </si>
+  <si>
+    <t>16:15 - 16:30</t>
+  </si>
+  <si>
+    <t>16:30 - 17:00</t>
+  </si>
+  <si>
+    <t>General discussion</t>
+  </si>
+  <si>
+    <t>(The other) dendroprovenancing: Developing ethical guidelines in dendrochronological research to protect cultural heritage</t>
+  </si>
+  <si>
+    <t>17:00 - 17:15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1286,6 +1286,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1368,7 +1374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1634,6 +1640,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1954,8 +1969,8 @@
   </sheetPr>
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2041,7 +2056,7 @@
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="26" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="6">
@@ -2077,7 +2092,7 @@
         <v>108</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="F7" s="55"/>
       <c r="G7" s="6">
@@ -2089,12 +2104,12 @@
         <v>11</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="57" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F8" s="55"/>
       <c r="G8" s="56">
@@ -2411,7 +2426,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -2563,7 +2578,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>113</v>
@@ -2601,7 +2616,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C32" s="48"/>
       <c r="D32" s="26"/>
@@ -2621,7 +2636,7 @@
         <v>92</v>
       </c>
       <c r="C33" s="86" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>94</v>
@@ -2630,7 +2645,7 @@
         <v>95</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="G33" s="6">
         <v>29</v>
@@ -2644,7 +2659,7 @@
         <v>96</v>
       </c>
       <c r="C34" s="86" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>101</v>
@@ -2653,7 +2668,7 @@
         <v>102</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="G34" s="56">
         <v>30</v>
@@ -2667,7 +2682,7 @@
         <v>100</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>97</v>
@@ -2690,13 +2705,13 @@
         <v>103</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E36" s="69" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>99</v>
@@ -2713,7 +2728,7 @@
         <v>106</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>104</v>
@@ -2736,7 +2751,7 @@
         <v>111</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>108</v>
@@ -2907,7 +2922,7 @@
         <v>11</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C46" s="70"/>
       <c r="D46" s="23"/>
@@ -2971,7 +2986,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>134</v>
@@ -2994,12 +3009,12 @@
         <v>11</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C50" s="71"/>
       <c r="D50" s="32"/>
       <c r="E50" s="72" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="56">
@@ -3011,7 +3026,7 @@
         <v>11</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -3037,7 +3052,7 @@
         <v>142</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C53" s="57"/>
       <c r="D53" s="57"/>
@@ -3408,7 +3423,7 @@
         <v>142</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C70" s="57"/>
       <c r="D70" s="57"/>
@@ -3618,7 +3633,7 @@
         <v>142</v>
       </c>
       <c r="B80" s="57" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C80" s="57"/>
       <c r="D80" s="57"/>
@@ -3791,7 +3806,7 @@
         <v>236</v>
       </c>
       <c r="B89" s="57" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C89" s="57"/>
       <c r="D89" s="57"/>
@@ -3811,7 +3826,7 @@
       <c r="C90" s="30"/>
       <c r="D90" s="26"/>
       <c r="E90" s="36" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="F90" s="30"/>
       <c r="G90" s="6">
@@ -3984,7 +3999,7 @@
         <v>236</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C98" s="34" t="s">
         <v>39</v>
@@ -4021,7 +4036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>236</v>
       </c>
@@ -4032,10 +4047,10 @@
         <v>262</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>263</v>
+        <v>365</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>264</v>
+        <v>327</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>194</v>
@@ -4044,120 +4059,120 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C101" s="33" t="s">
-        <v>265</v>
+      <c r="C101" s="29" t="s">
+        <v>302</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>371</v>
+        <v>300</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>194</v>
+        <v>340</v>
       </c>
       <c r="G101" s="88">
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="29" t="s">
-        <v>305</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="E102" s="19" t="s">
+      <c r="C102" s="14" t="s">
         <v>304</v>
       </c>
+      <c r="D102" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="E102" s="20" t="s">
+        <v>284</v>
+      </c>
       <c r="F102" s="14" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G102" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B103" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="D103" s="20" t="s">
-        <v>286</v>
-      </c>
-      <c r="E103" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="F103" s="14" t="s">
-        <v>346</v>
-      </c>
+      <c r="B103" s="66" t="s">
+        <v>353</v>
+      </c>
+      <c r="C103" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" s="68"/>
+      <c r="E103" s="62"/>
+      <c r="F103" s="82"/>
       <c r="G103" s="88">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B104" s="66" t="s">
-        <v>359</v>
-      </c>
-      <c r="C104" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="D104" s="68"/>
-      <c r="E104" s="62"/>
-      <c r="F104" s="82"/>
+      <c r="B104" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="C104" s="57"/>
+      <c r="D104" s="57"/>
+      <c r="E104" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="F104" s="57"/>
       <c r="G104" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B105" s="57" t="s">
-        <v>343</v>
-      </c>
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
-      <c r="E105" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="F105" s="57"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="F105" s="15"/>
       <c r="G105" s="88">
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B106" s="25"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="36" t="s">
+      <c r="B106" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E106" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="F106" s="15"/>
+      <c r="F106" s="9" t="s">
+        <v>339</v>
+      </c>
       <c r="G106" s="6">
         <v>18</v>
       </c>
@@ -4167,19 +4182,19 @@
         <v>236</v>
       </c>
       <c r="B107" s="37" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>93</v>
+        <v>338</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>291</v>
+        <v>312</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G107" s="88">
         <v>19</v>
@@ -4190,19 +4205,19 @@
         <v>236</v>
       </c>
       <c r="B108" s="37" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>344</v>
+        <v>266</v>
       </c>
       <c r="D108" s="7" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G108" s="6">
         <v>20</v>
@@ -4213,7 +4228,7 @@
         <v>236</v>
       </c>
       <c r="B109" s="37" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C109" s="9" t="s">
         <v>269</v>
@@ -4225,7 +4240,7 @@
         <v>295</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G109" s="88">
         <v>21</v>
@@ -4236,7 +4251,7 @@
         <v>236</v>
       </c>
       <c r="B110" s="37" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C110" s="9" t="s">
         <v>272</v>
@@ -4248,51 +4263,51 @@
         <v>298</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G110" s="6">
         <v>22</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B111" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="E111" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>345</v>
+      <c r="B111" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="C111" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="26"/>
+      <c r="E111" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>342</v>
       </c>
       <c r="G111" s="88">
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B112" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="C112" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D112" s="26"/>
-      <c r="E112" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F112" s="30" t="s">
-        <v>348</v>
+      <c r="B112" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C112" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="F112" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="G112" s="6">
         <v>24</v>
@@ -4306,16 +4321,16 @@
         <v>41</v>
       </c>
       <c r="C113" s="29" t="s">
-        <v>266</v>
+        <v>299</v>
       </c>
       <c r="D113" s="19" t="s">
-        <v>177</v>
+        <v>241</v>
       </c>
       <c r="E113" s="19" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>220</v>
+        <v>339</v>
       </c>
       <c r="G113" s="88">
         <v>25</v>
@@ -4329,22 +4344,22 @@
         <v>41</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>302</v>
+        <v>354</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>241</v>
+        <v>305</v>
       </c>
       <c r="E114" s="19" t="s">
         <v>306</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G114" s="6">
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>236</v>
       </c>
@@ -4352,22 +4367,22 @@
         <v>41</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D115" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="E115" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="E115" s="19" t="s">
-        <v>309</v>
-      </c>
       <c r="F115" s="14" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G115" s="88">
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>236</v>
       </c>
@@ -4375,145 +4390,145 @@
         <v>41</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D116" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="E116" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="E116" s="19" t="s">
-        <v>311</v>
-      </c>
       <c r="F116" s="14" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="G116" s="6">
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B117" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C117" s="29" t="s">
-        <v>362</v>
-      </c>
-      <c r="D117" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="F117" s="14" t="s">
-        <v>345</v>
-      </c>
+      <c r="B117" s="66" t="s">
+        <v>323</v>
+      </c>
+      <c r="C117" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="D117" s="81"/>
+      <c r="E117" s="80"/>
+      <c r="F117" s="63"/>
       <c r="G117" s="88">
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B118" s="66" t="s">
-        <v>327</v>
-      </c>
-      <c r="C118" s="80" t="s">
-        <v>90</v>
-      </c>
-      <c r="D118" s="81"/>
-      <c r="E118" s="80"/>
-      <c r="F118" s="63"/>
+      <c r="B118" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="C118" s="57"/>
+      <c r="D118" s="57"/>
+      <c r="E118" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="F118" s="57"/>
       <c r="G118" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B119" s="57" t="s">
-        <v>347</v>
-      </c>
-      <c r="C119" s="57"/>
-      <c r="D119" s="57"/>
-      <c r="E119" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="F119" s="57"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="F119" s="15"/>
       <c r="G119" s="88">
         <v>31</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B120" s="25"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="26"/>
-      <c r="E120" s="36" t="s">
+      <c r="B120" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E120" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="F120" s="15"/>
-      <c r="G120" s="88">
+      <c r="F120" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G120" s="6">
         <v>32</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B121" s="10" t="s">
-        <v>92</v>
+      <c r="B121" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>290</v>
       </c>
       <c r="D121" s="7" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="G121" s="6">
+        <v>340</v>
+      </c>
+      <c r="G121" s="88">
         <v>33</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B122" s="6" t="s">
-        <v>96</v>
+      <c r="B122" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>293</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="G122" s="88">
+        <v>340</v>
+      </c>
+      <c r="G122" s="6">
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>296</v>
@@ -4525,112 +4540,112 @@
         <v>274</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="G123" s="6">
+        <v>340</v>
+      </c>
+      <c r="G123" s="88">
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="D124" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E124" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="E124" s="7" t="s">
-        <v>277</v>
-      </c>
       <c r="F124" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="G124" s="88">
+        <v>340</v>
+      </c>
+      <c r="G124" s="6">
         <v>36</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>236</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>314</v>
       </c>
       <c r="D125" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E125" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E125" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="F125" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="G125" s="6">
+        <v>340</v>
+      </c>
+      <c r="G125" s="88">
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B126" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="F126" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="G126" s="88">
+      <c r="B126" s="59" t="s">
+        <v>324</v>
+      </c>
+      <c r="C126" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="D126" s="68"/>
+      <c r="E126" s="62"/>
+      <c r="F126" s="63"/>
+      <c r="G126" s="6">
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B127" s="59" t="s">
-        <v>328</v>
-      </c>
-      <c r="C127" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="D127" s="68"/>
-      <c r="E127" s="62"/>
-      <c r="F127" s="63"/>
-      <c r="G127" s="6">
+      <c r="B127" s="48" t="s">
+        <v>362</v>
+      </c>
+      <c r="C127" s="48"/>
+      <c r="D127" s="31"/>
+      <c r="E127" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="F127" s="15"/>
+      <c r="G127" s="88">
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B128" s="48" t="s">
-        <v>368</v>
-      </c>
-      <c r="C128" s="48"/>
-      <c r="D128" s="31"/>
-      <c r="E128" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="F128" s="15"/>
-      <c r="G128" s="88">
+      <c r="B128" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="G128" s="6">
         <v>40</v>
       </c>
     </row>
@@ -4639,19 +4654,19 @@
         <v>236</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G129" s="88">
         <v>41</v>
@@ -4661,94 +4676,90 @@
       <c r="A130" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B130" s="6" t="s">
-        <v>137</v>
+      <c r="B130" s="10" t="s">
+        <v>318</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>282</v>
+        <v>315</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>283</v>
+        <v>316</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G130" s="6">
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B131" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="F131" s="9" t="s">
-        <v>346</v>
-      </c>
+      <c r="B131" s="48"/>
+      <c r="C131" s="48"/>
+      <c r="D131" s="31"/>
+      <c r="E131" s="48" t="s">
+        <v>366</v>
+      </c>
+      <c r="F131" s="15"/>
       <c r="G131" s="88">
         <v>43</v>
       </c>
     </row>
-    <row r="132" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" s="91" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B132" s="48"/>
-      <c r="C132" s="48"/>
-      <c r="D132" s="31"/>
-      <c r="E132" s="48" t="s">
+      <c r="B132" s="91" t="s">
+        <v>369</v>
+      </c>
+      <c r="C132" s="92"/>
+      <c r="D132" s="38" t="s">
+        <v>368</v>
+      </c>
+      <c r="E132" s="90" t="s">
         <v>372</v>
       </c>
-      <c r="F132" s="15"/>
+      <c r="F132" s="9"/>
       <c r="G132" s="6">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B133" s="43" t="s">
-        <v>329</v>
+      <c r="B133" s="27" t="s">
+        <v>370</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="G133" s="88">
+        <v>371</v>
+      </c>
+      <c r="G133" s="6">
         <v>45</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="B134" s="43" t="s">
-        <v>330</v>
+      <c r="B134" s="27" t="s">
+        <v>373</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="G134" s="6">
+        <v>325</v>
+      </c>
+      <c r="G134" s="88">
         <v>46</v>
       </c>
     </row>
@@ -4757,15 +4768,15 @@
         <v>236</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C135" s="23"/>
       <c r="D135" s="18"/>
       <c r="E135" s="26" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F135" s="15"/>
-      <c r="G135" s="88">
+      <c r="G135" s="6">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change of chairs for session 5
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3DF11F-2D83-4CD0-B82D-51E523227FEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E76B180-9E2F-4283-B8BA-F742BDF54832}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -758,9 +758,6 @@
     <t>Sourcing timber in a historic war zone: The South East Scotland Oak Dendrochronology project</t>
   </si>
   <si>
-    <t>EXCURSIONS</t>
-  </si>
-  <si>
     <t>Thursday 21 April 2022</t>
   </si>
   <si>
@@ -1154,9 +1151,6 @@
     <t>Closing session</t>
   </si>
   <si>
-    <t>(chair: tba)</t>
-  </si>
-  <si>
     <t>Brita Lorentzen</t>
   </si>
   <si>
@@ -1187,13 +1181,19 @@
     <t>15:00 - 15:15</t>
   </si>
   <si>
-    <t>15:15 - 17:30</t>
-  </si>
-  <si>
     <t>S8-O-001</t>
   </si>
   <si>
     <t>Protective symbols applied by  craftsmen on worked timber during the 16th and 17th centuries, and some reasons for their application</t>
+  </si>
+  <si>
+    <t>(chair:  Jørgen Wadum)</t>
+  </si>
+  <si>
+    <t>15:15 - 19:00</t>
+  </si>
+  <si>
+    <t>EXCURSIONS (boat trip on the Amsterdam canals, ...)</t>
   </si>
 </sst>
 </file>
@@ -1978,8 +1978,8 @@
   </sheetPr>
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B83" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2065,7 +2065,7 @@
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="6">
@@ -2101,7 +2101,7 @@
         <v>108</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F7" s="55"/>
       <c r="G7" s="6">
@@ -2113,12 +2113,12 @@
         <v>11</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="57" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F8" s="55"/>
       <c r="G8" s="56">
@@ -2435,7 +2435,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -2587,7 +2587,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>113</v>
@@ -2625,7 +2625,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C32" s="48"/>
       <c r="D32" s="26"/>
@@ -2645,7 +2645,7 @@
         <v>92</v>
       </c>
       <c r="C33" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>94</v>
@@ -2654,7 +2654,7 @@
         <v>95</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G33" s="6">
         <v>29</v>
@@ -2668,7 +2668,7 @@
         <v>96</v>
       </c>
       <c r="C34" s="86" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>101</v>
@@ -2677,7 +2677,7 @@
         <v>102</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G34" s="56">
         <v>30</v>
@@ -2691,7 +2691,7 @@
         <v>100</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>97</v>
@@ -2714,13 +2714,13 @@
         <v>103</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E36" s="69" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>99</v>
@@ -2737,7 +2737,7 @@
         <v>106</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>104</v>
@@ -2760,7 +2760,7 @@
         <v>111</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>108</v>
@@ -2931,7 +2931,7 @@
         <v>11</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C46" s="70"/>
       <c r="D46" s="23"/>
@@ -2995,7 +2995,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>134</v>
@@ -3018,12 +3018,12 @@
         <v>11</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C50" s="71"/>
       <c r="D50" s="32"/>
       <c r="E50" s="72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="56">
@@ -3035,7 +3035,7 @@
         <v>11</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -3061,7 +3061,7 @@
         <v>142</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C53" s="57"/>
       <c r="D53" s="57"/>
@@ -3432,7 +3432,7 @@
         <v>142</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C70" s="57"/>
       <c r="D70" s="57"/>
@@ -3642,7 +3642,7 @@
         <v>142</v>
       </c>
       <c r="B80" s="57" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C80" s="57"/>
       <c r="D80" s="57"/>
@@ -3662,7 +3662,7 @@
       <c r="C81" s="26"/>
       <c r="D81" s="26"/>
       <c r="E81" s="36" t="s">
-        <v>216</v>
+        <v>376</v>
       </c>
       <c r="F81" s="15"/>
       <c r="G81" s="87">
@@ -3680,10 +3680,10 @@
         <v>107</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>220</v>
@@ -3789,16 +3789,16 @@
         <v>142</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>230</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="F87" s="9" t="s">
         <v>220</v>
@@ -3812,12 +3812,12 @@
         <v>142</v>
       </c>
       <c r="B88" s="85" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C88" s="55"/>
       <c r="D88" s="55"/>
       <c r="E88" s="55" t="s">
-        <v>233</v>
+        <v>378</v>
       </c>
       <c r="F88" s="50"/>
       <c r="G88" s="88">
@@ -3826,7 +3826,7 @@
     </row>
     <row r="89" spans="1:7" s="58" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C89" s="75"/>
       <c r="D89" s="83"/>
@@ -3835,10 +3835,10 @@
     </row>
     <row r="90" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B90" s="57" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C90" s="57"/>
       <c r="D90" s="57"/>
@@ -3852,13 +3852,13 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B91" s="25"/>
       <c r="C91" s="30"/>
       <c r="D91" s="26"/>
       <c r="E91" s="36" t="s">
-        <v>365</v>
+        <v>216</v>
       </c>
       <c r="F91" s="30"/>
       <c r="G91" s="6">
@@ -3867,19 +3867,19 @@
     </row>
     <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>145</v>
       </c>
       <c r="C92" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="E92" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="F92" s="9" t="s">
         <v>220</v>
@@ -3890,19 +3890,19 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B93" s="10" t="s">
         <v>150</v>
       </c>
       <c r="C93" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D93" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="E93" s="7" t="s">
         <v>240</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>241</v>
       </c>
       <c r="F93" s="9" t="s">
         <v>220</v>
@@ -3913,19 +3913,19 @@
     </row>
     <row r="94" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B94" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D94" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="E94" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>244</v>
       </c>
       <c r="F94" s="9" t="s">
         <v>220</v>
@@ -3936,19 +3936,19 @@
     </row>
     <row r="95" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C95" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D95" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="E95" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="F95" s="9" t="s">
         <v>220</v>
@@ -3959,19 +3959,19 @@
     </row>
     <row r="96" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C96" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D96" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="E96" s="7" t="s">
         <v>249</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>250</v>
       </c>
       <c r="F96" s="9" t="s">
         <v>220</v>
@@ -3982,19 +3982,19 @@
     </row>
     <row r="97" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C97" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D97" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D97" s="7" t="s">
+      <c r="E97" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>253</v>
       </c>
       <c r="F97" s="9" t="s">
         <v>220</v>
@@ -4003,21 +4003,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="F98" s="9" t="s">
         <v>220</v>
@@ -4028,10 +4028,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C99" s="34" t="s">
         <v>39</v>
@@ -4047,19 +4047,19 @@
     </row>
     <row r="100" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C100" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="D100" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="D100" s="19" t="s">
+      <c r="E100" s="19" t="s">
         <v>259</v>
-      </c>
-      <c r="E100" s="19" t="s">
-        <v>260</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>194</v>
@@ -4070,19 +4070,19 @@
     </row>
     <row r="101" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C101" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F101" s="14" t="s">
         <v>194</v>
@@ -4093,22 +4093,22 @@
     </row>
     <row r="102" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C102" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D102" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="E102" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="E102" s="19" t="s">
-        <v>300</v>
-      </c>
       <c r="F102" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G102" s="88">
         <v>13</v>
@@ -4116,22 +4116,22 @@
     </row>
     <row r="103" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B103" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D103" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="E103" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="E103" s="20" t="s">
-        <v>283</v>
-      </c>
       <c r="F103" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G103" s="6">
         <v>14</v>
@@ -4139,10 +4139,10 @@
     </row>
     <row r="104" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B104" s="66" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C104" s="67" t="s">
         <v>61</v>
@@ -4156,15 +4156,15 @@
     </row>
     <row r="105" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B105" s="57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C105" s="57"/>
       <c r="D105" s="57"/>
       <c r="E105" s="57" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F105" s="57"/>
       <c r="G105" s="6">
@@ -4173,13 +4173,13 @@
     </row>
     <row r="106" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B106" s="25"/>
       <c r="C106" s="26"/>
       <c r="D106" s="26"/>
       <c r="E106" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F106" s="15"/>
       <c r="G106" s="88">
@@ -4188,7 +4188,7 @@
     </row>
     <row r="107" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B107" s="37" t="s">
         <v>64</v>
@@ -4197,13 +4197,13 @@
         <v>93</v>
       </c>
       <c r="D107" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E107" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="E107" s="7" t="s">
-        <v>288</v>
-      </c>
       <c r="F107" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G107" s="6">
         <v>18</v>
@@ -4211,45 +4211,45 @@
     </row>
     <row r="108" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B108" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C108" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="F108" s="9" t="s">
         <v>336</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>337</v>
       </c>
       <c r="G108" s="88">
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B109" s="37" t="s">
         <v>73</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D109" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="E109" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="E109" s="7" t="s">
-        <v>291</v>
-      </c>
       <c r="F109" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G109" s="6">
         <v>20</v>
@@ -4257,22 +4257,22 @@
     </row>
     <row r="110" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B110" s="37" t="s">
         <v>77</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D110" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E110" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="E110" s="7" t="s">
-        <v>294</v>
-      </c>
       <c r="F110" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G110" s="88">
         <v>21</v>
@@ -4280,22 +4280,22 @@
     </row>
     <row r="111" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B111" s="37" t="s">
         <v>81</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D111" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="E111" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="E111" s="7" t="s">
-        <v>297</v>
-      </c>
       <c r="F111" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G111" s="6">
         <v>22</v>
@@ -4303,10 +4303,10 @@
     </row>
     <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C112" s="34" t="s">
         <v>39</v>
@@ -4316,7 +4316,7 @@
         <v>40</v>
       </c>
       <c r="F112" s="30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G112" s="88">
         <v>23</v>
@@ -4324,19 +4324,19 @@
     </row>
     <row r="113" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B113" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C113" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D113" s="19" t="s">
         <v>177</v>
       </c>
       <c r="E113" s="19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F113" s="14" t="s">
         <v>220</v>
@@ -4347,22 +4347,22 @@
     </row>
     <row r="114" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B114" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G114" s="88">
         <v>25</v>
@@ -4370,22 +4370,22 @@
     </row>
     <row r="115" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B115" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D115" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="E115" s="19" t="s">
         <v>304</v>
       </c>
-      <c r="E115" s="19" t="s">
-        <v>305</v>
-      </c>
       <c r="F115" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G115" s="6">
         <v>26</v>
@@ -4393,22 +4393,22 @@
     </row>
     <row r="116" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B116" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D116" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="E116" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="E116" s="19" t="s">
-        <v>307</v>
-      </c>
       <c r="F116" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G116" s="88">
         <v>27</v>
@@ -4416,22 +4416,22 @@
     </row>
     <row r="117" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B117" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C117" s="29" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D117" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="E117" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="E117" s="19" t="s">
-        <v>309</v>
-      </c>
       <c r="F117" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G117" s="6">
         <v>28</v>
@@ -4439,10 +4439,10 @@
     </row>
     <row r="118" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B118" s="66" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C118" s="80" t="s">
         <v>90</v>
@@ -4456,15 +4456,15 @@
     </row>
     <row r="119" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B119" s="57" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C119" s="57"/>
       <c r="D119" s="57"/>
       <c r="E119" s="57" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F119" s="57"/>
       <c r="G119" s="6">
@@ -4473,13 +4473,13 @@
     </row>
     <row r="120" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B120" s="25"/>
       <c r="C120" s="26"/>
       <c r="D120" s="26"/>
       <c r="E120" s="36" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F120" s="15"/>
       <c r="G120" s="88">
@@ -4488,22 +4488,22 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B121" s="10" t="s">
         <v>92</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D121" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E121" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="E121" s="7" t="s">
-        <v>267</v>
-      </c>
       <c r="F121" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G121" s="6">
         <v>32</v>
@@ -4511,22 +4511,22 @@
     </row>
     <row r="122" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D122" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E122" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="E122" s="7" t="s">
-        <v>257</v>
-      </c>
       <c r="F122" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G122" s="88">
         <v>33</v>
@@ -4534,22 +4534,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B123" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D123" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E123" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="E123" s="7" t="s">
-        <v>270</v>
-      </c>
       <c r="F123" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G123" s="6">
         <v>34</v>
@@ -4557,22 +4557,22 @@
     </row>
     <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B124" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D124" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E124" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="E124" s="7" t="s">
-        <v>273</v>
-      </c>
       <c r="F124" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G124" s="88">
         <v>35</v>
@@ -4580,22 +4580,22 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B125" s="10" t="s">
         <v>106</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D125" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E125" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="E125" s="7" t="s">
-        <v>275</v>
-      </c>
       <c r="F125" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G125" s="6">
         <v>36</v>
@@ -4603,22 +4603,22 @@
     </row>
     <row r="126" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B126" s="10" t="s">
         <v>111</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D126" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E126" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="E126" s="7" t="s">
-        <v>277</v>
-      </c>
       <c r="F126" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G126" s="88">
         <v>37</v>
@@ -4626,10 +4626,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B127" s="59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C127" s="67" t="s">
         <v>61</v>
@@ -4643,15 +4643,15 @@
     </row>
     <row r="128" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B128" s="48" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C128" s="48"/>
       <c r="D128" s="31"/>
       <c r="E128" s="57" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F128" s="15"/>
       <c r="G128" s="88">
@@ -4660,22 +4660,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D129" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E129" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="E129" s="7" t="s">
-        <v>281</v>
-      </c>
       <c r="F129" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G129" s="6">
         <v>40</v>
@@ -4683,22 +4683,22 @@
     </row>
     <row r="130" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>137</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D130" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E130" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="E130" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="F130" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G130" s="88">
         <v>41</v>
@@ -4706,22 +4706,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D131" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="E131" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="E131" s="7" t="s">
-        <v>315</v>
-      </c>
       <c r="F131" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G131" s="6">
         <v>42</v>
@@ -4729,13 +4729,13 @@
     </row>
     <row r="132" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B132" s="48"/>
       <c r="C132" s="48"/>
       <c r="D132" s="31"/>
       <c r="E132" s="48" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F132" s="15"/>
       <c r="G132" s="88">
@@ -4744,19 +4744,19 @@
     </row>
     <row r="133" spans="1:7" s="91" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B133" s="91" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C133" s="92" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D133" s="38" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E133" s="90" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F133" s="9"/>
       <c r="G133" s="6">
@@ -4765,16 +4765,16 @@
     </row>
     <row r="134" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G134" s="6">
         <v>45</v>
@@ -4782,16 +4782,16 @@
     </row>
     <row r="135" spans="1:7" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B135" s="27" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E135" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G135" s="88">
         <v>46</v>
@@ -4799,15 +4799,15 @@
     </row>
     <row r="136" spans="1:7" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C136" s="23"/>
       <c r="D136" s="18"/>
       <c r="E136" s="26" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F136" s="15"/>
       <c r="G136" s="6">

</xml_diff>

<commit_message>
presenter Tamar changed to Frederickx
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28380914-39D3-4490-BA19-73C8B240B9AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC33D53-0AE7-47E7-A751-8A04C11FC5D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -983,9 +983,6 @@
     <t>S7-O-005</t>
   </si>
   <si>
-    <t>Tamar Hestrin-Grader</t>
-  </si>
-  <si>
     <t>Old and new, large and small: Non-invasive techniques applied to a musical instrument</t>
   </si>
   <si>
@@ -1194,13 +1191,16 @@
   </si>
   <si>
     <t>REGISTRATION &amp; ICEBREAKER (and hanging of posters)</t>
+  </si>
+  <si>
+    <t>Manu Frederickx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1301,6 +1301,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1383,7 +1389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1659,6 +1665,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1978,8 +1985,8 @@
   </sheetPr>
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2033,12 +2040,12 @@
         <v>7</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="6">
@@ -2065,7 +2072,7 @@
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="6">
@@ -2101,7 +2108,7 @@
         <v>106</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F7" s="55"/>
       <c r="G7" s="6">
@@ -2113,12 +2120,12 @@
         <v>9</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="57" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F8" s="55"/>
       <c r="G8" s="56">
@@ -2435,7 +2442,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C23" s="57"/>
       <c r="D23" s="57"/>
@@ -2587,7 +2594,7 @@
         <v>83</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>111</v>
@@ -2625,7 +2632,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="48" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C32" s="48"/>
       <c r="D32" s="26"/>
@@ -2645,7 +2652,7 @@
         <v>90</v>
       </c>
       <c r="C33" s="86" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>92</v>
@@ -2654,7 +2661,7 @@
         <v>93</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G33" s="6">
         <v>29</v>
@@ -2668,7 +2675,7 @@
         <v>94</v>
       </c>
       <c r="C34" s="86" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>99</v>
@@ -2677,7 +2684,7 @@
         <v>100</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G34" s="56">
         <v>30</v>
@@ -2691,7 +2698,7 @@
         <v>98</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>95</v>
@@ -2714,13 +2721,13 @@
         <v>101</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E36" s="69" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>97</v>
@@ -2737,7 +2744,7 @@
         <v>104</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>102</v>
@@ -2760,7 +2767,7 @@
         <v>109</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>106</v>
@@ -2931,7 +2938,7 @@
         <v>9</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C46" s="70"/>
       <c r="D46" s="23"/>
@@ -2995,7 +3002,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>132</v>
@@ -3018,12 +3025,12 @@
         <v>9</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C50" s="71"/>
       <c r="D50" s="32"/>
       <c r="E50" s="72" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="56">
@@ -3035,7 +3042,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -3061,7 +3068,7 @@
         <v>140</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C53" s="57"/>
       <c r="D53" s="57"/>
@@ -3432,7 +3439,7 @@
         <v>140</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C70" s="57"/>
       <c r="D70" s="57"/>
@@ -3642,7 +3649,7 @@
         <v>140</v>
       </c>
       <c r="B80" s="57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C80" s="57"/>
       <c r="D80" s="57"/>
@@ -3662,7 +3669,7 @@
       <c r="C81" s="26"/>
       <c r="D81" s="26"/>
       <c r="E81" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F81" s="15"/>
       <c r="G81" s="87">
@@ -3680,10 +3687,10 @@
         <v>105</v>
       </c>
       <c r="D82" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E82" s="7" t="s">
         <v>368</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>369</v>
       </c>
       <c r="F82" s="9" t="s">
         <v>218</v>
@@ -3789,7 +3796,7 @@
         <v>140</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>228</v>
@@ -3812,12 +3819,12 @@
         <v>140</v>
       </c>
       <c r="B88" s="85" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C88" s="55"/>
       <c r="D88" s="55"/>
       <c r="E88" s="55" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F88" s="50"/>
       <c r="G88" s="88">
@@ -3838,7 +3845,7 @@
         <v>232</v>
       </c>
       <c r="B90" s="57" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C90" s="57"/>
       <c r="D90" s="57"/>
@@ -4011,7 +4018,7 @@
         <v>28</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>229</v>
@@ -4031,7 +4038,7 @@
         <v>232</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C99" s="34" t="s">
         <v>37</v>
@@ -4079,10 +4086,10 @@
         <v>258</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F101" s="14" t="s">
         <v>192</v>
@@ -4108,7 +4115,7 @@
         <v>297</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G102" s="88">
         <v>13</v>
@@ -4131,7 +4138,7 @@
         <v>280</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G103" s="6">
         <v>14</v>
@@ -4142,7 +4149,7 @@
         <v>232</v>
       </c>
       <c r="B104" s="66" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C104" s="67" t="s">
         <v>59</v>
@@ -4159,7 +4166,7 @@
         <v>232</v>
       </c>
       <c r="B105" s="57" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C105" s="57"/>
       <c r="D105" s="57"/>
@@ -4203,13 +4210,13 @@
         <v>285</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G107" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.4">
       <c r="A108" s="6" t="s">
         <v>232</v>
       </c>
@@ -4217,22 +4224,22 @@
         <v>67</v>
       </c>
       <c r="C108" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D108" s="93" t="s">
+        <v>378</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="F108" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>334</v>
       </c>
       <c r="G108" s="88">
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>232</v>
       </c>
@@ -4249,7 +4256,7 @@
         <v>288</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G109" s="6">
         <v>20</v>
@@ -4272,7 +4279,7 @@
         <v>291</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G110" s="88">
         <v>21</v>
@@ -4295,7 +4302,7 @@
         <v>294</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G111" s="6">
         <v>22</v>
@@ -4306,7 +4313,7 @@
         <v>232</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C112" s="34" t="s">
         <v>37</v>
@@ -4316,7 +4323,7 @@
         <v>38</v>
       </c>
       <c r="F112" s="30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G112" s="88">
         <v>23</v>
@@ -4362,7 +4369,7 @@
         <v>299</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G114" s="88">
         <v>25</v>
@@ -4376,7 +4383,7 @@
         <v>39</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D115" s="19" t="s">
         <v>301</v>
@@ -4385,7 +4392,7 @@
         <v>302</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G115" s="6">
         <v>26</v>
@@ -4399,7 +4406,7 @@
         <v>39</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>303</v>
@@ -4408,7 +4415,7 @@
         <v>304</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G116" s="88">
         <v>27</v>
@@ -4422,7 +4429,7 @@
         <v>39</v>
       </c>
       <c r="C117" s="29" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D117" s="19" t="s">
         <v>305</v>
@@ -4431,7 +4438,7 @@
         <v>306</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G117" s="6">
         <v>28</v>
@@ -4442,7 +4449,7 @@
         <v>232</v>
       </c>
       <c r="B118" s="66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C118" s="80" t="s">
         <v>88</v>
@@ -4459,7 +4466,7 @@
         <v>232</v>
       </c>
       <c r="B119" s="57" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C119" s="57"/>
       <c r="D119" s="57"/>
@@ -4503,7 +4510,7 @@
         <v>264</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G121" s="6">
         <v>32</v>
@@ -4526,7 +4533,7 @@
         <v>254</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G122" s="88">
         <v>33</v>
@@ -4549,7 +4556,7 @@
         <v>267</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G123" s="6">
         <v>34</v>
@@ -4572,7 +4579,7 @@
         <v>270</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G124" s="88">
         <v>35</v>
@@ -4595,7 +4602,7 @@
         <v>272</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G125" s="6">
         <v>36</v>
@@ -4609,7 +4616,7 @@
         <v>109</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>273</v>
@@ -4618,7 +4625,7 @@
         <v>274</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G126" s="88">
         <v>37</v>
@@ -4629,7 +4636,7 @@
         <v>232</v>
       </c>
       <c r="B127" s="59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C127" s="67" t="s">
         <v>59</v>
@@ -4646,7 +4653,7 @@
         <v>232</v>
       </c>
       <c r="B128" s="48" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C128" s="48"/>
       <c r="D128" s="31"/>
@@ -4666,7 +4673,7 @@
         <v>131</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>277</v>
@@ -4675,7 +4682,7 @@
         <v>278</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G129" s="6">
         <v>40</v>
@@ -4689,7 +4696,7 @@
         <v>135</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>275</v>
@@ -4698,7 +4705,7 @@
         <v>276</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G130" s="88">
         <v>41</v>
@@ -4709,19 +4716,19 @@
         <v>232</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D131" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="E131" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="E131" s="7" t="s">
-        <v>312</v>
-      </c>
       <c r="F131" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G131" s="6">
         <v>42</v>
@@ -4735,7 +4742,7 @@
       <c r="C132" s="48"/>
       <c r="D132" s="31"/>
       <c r="E132" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F132" s="15"/>
       <c r="G132" s="88">
@@ -4747,16 +4754,16 @@
         <v>232</v>
       </c>
       <c r="B133" s="91" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C133" s="92" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D133" s="38" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E133" s="90" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F133" s="9"/>
       <c r="G133" s="6">
@@ -4768,13 +4775,13 @@
         <v>232</v>
       </c>
       <c r="B134" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="D134" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E134" s="9" t="s">
         <v>364</v>
-      </c>
-      <c r="D134" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>365</v>
       </c>
       <c r="G134" s="6">
         <v>45</v>
@@ -4785,13 +4792,13 @@
         <v>232</v>
       </c>
       <c r="B135" s="27" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>13</v>
       </c>
       <c r="E135" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G135" s="88">
         <v>46</v>
@@ -4802,12 +4809,12 @@
         <v>232</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C136" s="23"/>
       <c r="D136" s="18"/>
       <c r="E136" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F136" s="15"/>
       <c r="G136" s="6">

</xml_diff>

<commit_message>
chair Belasus moved to second part
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC33D53-0AE7-47E7-A751-8A04C11FC5D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E55C7FA-1A24-4735-84D4-F2D33809F7AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="380">
   <si>
     <t>day</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Monday 18/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:00 - 20:00 </t>
+  </si>
+  <si>
+    <t>REGISTRATION &amp; ICEBREAKER</t>
   </si>
   <si>
     <t>Tuesday 19 April 2022</t>
@@ -827,9 +833,6 @@
     <t>S4-P-001</t>
   </si>
   <si>
-    <t>Andreas Rais</t>
-  </si>
-  <si>
     <t>Mechanical wood properties over the past 100 years</t>
   </si>
   <si>
@@ -1031,9 +1034,6 @@
     <t>S7-O-008</t>
   </si>
   <si>
-    <t>S7-O-009</t>
-  </si>
-  <si>
     <t>Session 2</t>
   </si>
   <si>
@@ -1172,9 +1172,6 @@
     <t>15:00 - 15:15</t>
   </si>
   <si>
-    <t>S8-O-001</t>
-  </si>
-  <si>
     <t>Protective symbols applied by  craftsmen on worked timber during the 16th and 17th centuries, and some reasons for their application</t>
   </si>
   <si>
@@ -1187,20 +1184,26 @@
     <t>EXCURSIONS (boat trip on the Amsterdam canals, ...)</t>
   </si>
   <si>
-    <t xml:space="preserve">17:00 - 20:00 </t>
-  </si>
-  <si>
-    <t>REGISTRATION &amp; ICEBREAKER (and hanging of posters)</t>
-  </si>
-  <si>
     <t>Manu Frederickx</t>
+  </si>
+  <si>
+    <t>(chair: Aoife Daly)</t>
+  </si>
+  <si>
+    <t>S7-PR-003</t>
+  </si>
+  <si>
+    <t>S8-PR-001</t>
+  </si>
+  <si>
+    <t>Jan-Willem G. van de Kuilen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1301,12 +1304,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1389,7 +1386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1509,19 +1506,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1665,7 +1653,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1983,10 +1970,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I151"/>
+  <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2010,7 +1997,7 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
@@ -2027,7 +2014,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="24"/>
@@ -2040,34 +2027,34 @@
         <v>7</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>376</v>
+        <v>8</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
       <c r="E3" s="26" t="s">
-        <v>377</v>
+        <v>9</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="6">
         <v>1</v>
       </c>
-      <c r="I3" s="46"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" spans="1:9" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="47"/>
+      <c r="B4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="44"/>
       <c r="D4" s="22"/>
       <c r="E4" s="17"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -2081,113 +2068,113 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="54"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="56">
+      <c r="C6" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="86" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="F7" s="55"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="54" t="s">
         <v>326</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="54" t="s">
         <v>327</v>
       </c>
-      <c r="F8" s="55"/>
-      <c r="G8" s="56">
+      <c r="F8" s="52"/>
+      <c r="G8" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
       <c r="E9" s="18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" s="15"/>
-      <c r="G9" s="6">
+      <c r="G9" s="53">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="56">
+        <v>21</v>
+      </c>
+      <c r="G10" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="G11" s="6">
         <v>7</v>
@@ -2195,45 +2182,45 @@
     </row>
     <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="56">
+        <v>21</v>
+      </c>
+      <c r="G12" s="53">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G13" s="6">
         <v>9</v>
@@ -2241,88 +2228,88 @@
     </row>
     <row r="14" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="56">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6">
         <v>10</v>
       </c>
       <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F15" s="30"/>
-      <c r="G15" s="6">
+      <c r="G15" s="53">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="56">
+        <v>21</v>
+      </c>
+      <c r="G16" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G17" s="6">
         <v>13</v>
@@ -2330,45 +2317,45 @@
     </row>
     <row r="18" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="56">
+        <v>21</v>
+      </c>
+      <c r="G18" s="53">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G19" s="6">
         <v>15</v>
@@ -2376,210 +2363,210 @@
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="56">
+        <v>21</v>
+      </c>
+      <c r="G20" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="6">
+        <v>21</v>
+      </c>
+      <c r="G21" s="53">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="56">
+        <v>11</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="58"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="6">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="54" t="s">
         <v>325</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="57"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="54"/>
       <c r="G23" s="6">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="35"/>
       <c r="D24" s="26"/>
       <c r="E24" s="18" t="s">
-        <v>61</v>
+        <v>376</v>
       </c>
       <c r="F24" s="35"/>
-      <c r="G24" s="56">
+      <c r="G24" s="53">
         <v>20</v>
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G25" s="6">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="56">
+      <c r="G26" s="6">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" s="6">
+        <v>68</v>
+      </c>
+      <c r="G27" s="53">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="56">
+        <v>68</v>
+      </c>
+      <c r="G28" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G29" s="6">
         <v>25</v>
@@ -2588,2267 +2575,2278 @@
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>328</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G30" s="56">
+        <v>115</v>
+      </c>
+      <c r="G30" s="53">
         <v>26</v>
       </c>
-      <c r="I30" s="65"/>
+      <c r="I30" s="62"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="66" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="68"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="63"/>
+        <v>11</v>
+      </c>
+      <c r="B31" s="63" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="65"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="6">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="45" t="s">
         <v>355</v>
       </c>
-      <c r="C32" s="48"/>
+      <c r="C32" s="45"/>
       <c r="D32" s="26"/>
       <c r="E32" s="30" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F32" s="15"/>
-      <c r="G32" s="56">
+      <c r="G32" s="6">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="86" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="83" t="s">
         <v>351</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="53">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="83" t="s">
         <v>352</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="G34" s="56">
+      <c r="G34" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C35" s="39" t="s">
         <v>339</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G35" s="6">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C36" s="39" t="s">
         <v>340</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="E36" s="69" t="s">
-        <v>372</v>
+        <v>315</v>
+      </c>
+      <c r="E36" s="66" t="s">
+        <v>371</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="56">
+        <v>99</v>
+      </c>
+      <c r="G36" s="53">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C37" s="39" t="s">
         <v>341</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G37" s="6">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B38" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="D38" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="39" t="s">
-        <v>315</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>107</v>
-      </c>
       <c r="F38" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" s="56">
+        <v>110</v>
+      </c>
+      <c r="G38" s="6">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C39" s="34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F39" s="30"/>
-      <c r="G39" s="6">
+      <c r="G39" s="53">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G40" s="56">
+        <v>68</v>
+      </c>
+      <c r="G40" s="6">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G41" s="6">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="56">
+        <v>68</v>
+      </c>
+      <c r="G42" s="53">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" s="9" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G43" s="6">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="9" customFormat="1" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" s="9" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G44" s="56">
+        <v>68</v>
+      </c>
+      <c r="G44" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="59" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="68"/>
-      <c r="E45" s="62"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="6">
+        <v>11</v>
+      </c>
+      <c r="B45" s="56" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="65"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="53">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="67" t="s">
         <v>342</v>
       </c>
-      <c r="C46" s="70"/>
+      <c r="C46" s="67"/>
       <c r="D46" s="23"/>
-      <c r="E46" s="57" t="s">
-        <v>60</v>
+      <c r="E46" s="54" t="s">
+        <v>62</v>
       </c>
       <c r="F46" s="15"/>
-      <c r="G46" s="56">
+      <c r="G46" s="6">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>66</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B47" s="67"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F47" s="15"/>
       <c r="G47" s="6">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G48" s="56">
+        <v>68</v>
+      </c>
+      <c r="G48" s="53">
         <v>44</v>
       </c>
-      <c r="I48" s="11"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>313</v>
+        <v>137</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D49" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>137</v>
-      </c>
       <c r="F49" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G49" s="6">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B50" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A51" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="48" t="s">
         <v>343</v>
       </c>
-      <c r="C50" s="71"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="72" t="s">
+      <c r="C51" s="68"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="69" t="s">
         <v>345</v>
       </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="56">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B51" s="51" t="s">
+      <c r="F51" s="13"/>
+      <c r="G51" s="53">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="6">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="9" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="73" t="s">
-        <v>139</v>
-      </c>
-      <c r="C52" s="74"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="77"/>
-    </row>
-    <row r="53" spans="1:9" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A53" s="9" t="s">
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B53" s="57" t="s">
+      <c r="F52" s="13"/>
+      <c r="G52" s="6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="9" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="70" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="71"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="74"/>
+    </row>
+    <row r="54" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="54" t="s">
         <v>329</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
-      <c r="E53" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="F53" s="57"/>
-      <c r="G53" s="88">
+      <c r="C54" s="54"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="54"/>
+      <c r="G54" s="85">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="36" t="s">
+    <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F54" s="15"/>
-      <c r="G54" s="87">
+      <c r="B55" s="25"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F55" s="15"/>
+      <c r="G55" s="84">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D55" s="7" t="s">
+    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A56" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="C56" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="D56" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="G55" s="88">
+      <c r="E56" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G56" s="85">
         <v>3</v>
       </c>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F57" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G56" s="87">
+      <c r="G57" s="84">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="E57" s="7" t="s">
+    <row r="58" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F57" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G57" s="88">
+      <c r="D58" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G58" s="85">
         <v>5</v>
       </c>
-      <c r="I57" s="46"/>
-    </row>
-    <row r="58" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E58" s="7" t="s">
+      <c r="I58" s="43"/>
+    </row>
+    <row r="59" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F58" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G58" s="87">
+      <c r="D59" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" s="84">
         <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A59" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G59" s="88">
-        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C60" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="E60" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="F60" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G60" s="85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="F60" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G60" s="87">
+      <c r="D61" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G61" s="84">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A61" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E61" s="7" t="s">
+    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A62" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F61" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G61" s="88">
+      <c r="D62" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" s="85">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E62" s="7" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F62" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="G62" s="87">
+      <c r="D63" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G63" s="84">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B63" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C63" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="D63" s="30"/>
-      <c r="E63" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F63" s="30"/>
-      <c r="G63" s="88">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B64" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C64" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="E64" s="20" t="s">
+      <c r="D64" s="30"/>
+      <c r="E64" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="30"/>
+      <c r="G64" s="85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="F64" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G64" s="87">
+      <c r="D65" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F65" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G65" s="84">
         <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A65" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B65" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>175</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="F65" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G65" s="88">
-        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C66" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D66" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="E66" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="E66" s="20" t="s">
+      <c r="F66" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G66" s="85">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="F66" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G66" s="87">
+      <c r="D67" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G67" s="84">
         <v>14</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B67" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E67" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F67" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G67" s="88">
-        <v>15</v>
-      </c>
-      <c r="I67" s="78"/>
     </row>
     <row r="68" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E68" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G68" s="85">
+        <v>15</v>
+      </c>
+      <c r="I68" s="75"/>
+    </row>
+    <row r="69" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C69" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F68" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G68" s="87">
+      <c r="D69" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F69" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G69" s="84">
         <v>16</v>
       </c>
-      <c r="I68" s="78"/>
-    </row>
-    <row r="69" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B69" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="C69" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="D69" s="67"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="63"/>
-      <c r="G69" s="88">
+    </row>
+    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" s="63" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="64"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="60"/>
+      <c r="G70" s="85">
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B70" s="57" t="s">
+    <row r="71" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" s="54" t="s">
         <v>330</v>
       </c>
-      <c r="C70" s="57"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="57" t="s">
-        <v>187</v>
-      </c>
-      <c r="F70" s="57"/>
-      <c r="G70" s="88">
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54" t="s">
+        <v>189</v>
+      </c>
+      <c r="F71" s="54"/>
+      <c r="G71" s="85">
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B71" s="25"/>
-      <c r="C71" s="53"/>
-      <c r="D71" s="53"/>
-      <c r="E71" s="79" t="s">
-        <v>188</v>
-      </c>
-      <c r="F71" s="50"/>
-      <c r="G71" s="87">
+    <row r="72" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="25"/>
+      <c r="C72" s="50"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="76" t="s">
+        <v>190</v>
+      </c>
+      <c r="F72" s="47"/>
+      <c r="G72" s="84">
         <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G72" s="88">
-        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C73" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="F73" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G73" s="88">
-        <v>21</v>
+      <c r="G73" s="85">
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="E74" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E74" s="5" t="s">
+      <c r="F74" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G74" s="85">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A75" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="F74" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G74" s="87">
+      <c r="D75" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G75" s="84">
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="E75" s="5" t="s">
+    <row r="76" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="F75" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G75" s="88">
+      <c r="D76" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G76" s="85">
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E76" s="7" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="F76" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G76" s="87">
+      <c r="D77" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G77" s="84">
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A77" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="E77" s="5" t="s">
+    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A78" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F77" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G77" s="88">
+      <c r="D78" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G78" s="85">
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A78" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="D78" s="6" t="s">
+    <row r="79" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="E78" s="5" t="s">
+      <c r="C79" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="F78" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="G78" s="87">
+      <c r="D79" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G79" s="84">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A79" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B79" s="66" t="s">
-        <v>212</v>
-      </c>
-      <c r="C79" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="D79" s="81"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="63"/>
-      <c r="G79" s="88">
+    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B80" s="63" t="s">
+        <v>214</v>
+      </c>
+      <c r="C80" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="D80" s="78"/>
+      <c r="E80" s="77"/>
+      <c r="F80" s="60"/>
+      <c r="G80" s="85">
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B80" s="57" t="s">
+    <row r="81" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B81" s="54" t="s">
         <v>358</v>
       </c>
-      <c r="C80" s="57"/>
-      <c r="D80" s="57"/>
-      <c r="E80" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="F80" s="57"/>
-      <c r="G80" s="88">
+      <c r="C81" s="54"/>
+      <c r="D81" s="54"/>
+      <c r="E81" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="F81" s="54"/>
+      <c r="G81" s="85">
         <v>28</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B81" s="25"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="26"/>
-      <c r="E81" s="36" t="s">
+    <row r="82" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="25"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="36" t="s">
+        <v>372</v>
+      </c>
+      <c r="F82" s="15"/>
+      <c r="G82" s="84">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G83" s="85">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G84" s="84">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G85" s="85">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G86" s="84">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G87" s="85">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G88" s="84">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="24.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B89" s="82" t="s">
         <v>373</v>
       </c>
-      <c r="F81" s="15"/>
-      <c r="G81" s="87">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A82" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G82" s="88">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A83" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C83" s="8" t="s">
+      <c r="C89" s="52"/>
+      <c r="D89" s="52"/>
+      <c r="E89" s="52" t="s">
+        <v>374</v>
+      </c>
+      <c r="F89" s="47"/>
+      <c r="G89" s="85">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" s="55" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="70" t="s">
+        <v>233</v>
+      </c>
+      <c r="C90" s="72"/>
+      <c r="D90" s="80"/>
+      <c r="E90" s="81"/>
+      <c r="F90" s="74"/>
+    </row>
+    <row r="91" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B91" s="54" t="s">
+        <v>357</v>
+      </c>
+      <c r="C91" s="54"/>
+      <c r="D91" s="54"/>
+      <c r="E91" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="F91" s="54"/>
+      <c r="G91" s="85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B92" s="25"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="E83" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G83" s="87">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A84" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="D84" s="7" t="s">
+      <c r="F92" s="30"/>
+      <c r="G92" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F93" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="E84" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G84" s="88">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G85" s="87">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A86" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G86" s="88">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G87" s="87">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="24.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B88" s="85" t="s">
-        <v>374</v>
-      </c>
-      <c r="C88" s="55"/>
-      <c r="D88" s="55"/>
-      <c r="E88" s="55" t="s">
-        <v>375</v>
-      </c>
-      <c r="F88" s="50"/>
-      <c r="G88" s="88">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" s="58" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="73" t="s">
-        <v>231</v>
-      </c>
-      <c r="C89" s="75"/>
-      <c r="D89" s="83"/>
-      <c r="E89" s="84"/>
-      <c r="F89" s="77"/>
-    </row>
-    <row r="90" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B90" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="C90" s="57"/>
-      <c r="D90" s="57"/>
-      <c r="E90" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="F90" s="57"/>
-      <c r="G90" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B91" s="25"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="F91" s="30"/>
-      <c r="G91" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A92" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B92" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D92" s="7" t="s">
+      <c r="G93" s="85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="E92" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G92" s="88">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E93" s="7" t="s">
+      <c r="B94" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="F93" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G93" s="6">
+      <c r="D94" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G94" s="6">
         <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B94" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G94" s="88">
-        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C95" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D95" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="E95" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="E95" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="F95" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G95" s="6">
-        <v>6</v>
+        <v>220</v>
+      </c>
+      <c r="G95" s="85">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G96" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G97" s="85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G98" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E99" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B96" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G96" s="88">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B97" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G97" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G98" s="88">
+      <c r="F99" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G99" s="85">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B99" s="25" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B100" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="C99" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D99" s="26"/>
-      <c r="E99" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F99" s="30"/>
-      <c r="G99" s="6">
+      <c r="C100" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100" s="26"/>
+      <c r="E100" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F100" s="30"/>
+      <c r="G100" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A100" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B100" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C100" s="33" t="s">
-        <v>255</v>
-      </c>
-      <c r="D100" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="E100" s="19" t="s">
+    <row r="101" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B101" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C101" s="33" t="s">
         <v>257</v>
       </c>
-      <c r="F100" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="G100" s="88">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B101" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C101" s="33" t="s">
+      <c r="D101" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="E101" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="D101" s="19" t="s">
+      <c r="F101" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="G101" s="85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B102" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C102" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="D102" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="E101" s="19" t="s">
-        <v>321</v>
-      </c>
-      <c r="F101" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="G101" s="6">
+      <c r="E102" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="G102" s="6">
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B102" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C102" s="29" t="s">
+    <row r="103" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B103" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C103" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="D103" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="E103" s="19" t="s">
         <v>298</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="E102" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="F102" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G102" s="88">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B103" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="D103" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="E103" s="20" t="s">
-        <v>280</v>
       </c>
       <c r="F103" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="G103" s="6">
+      <c r="G103" s="85">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B104" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="D104" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="E104" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="F104" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="G104" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A104" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B104" s="66" t="s">
+    <row r="105" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A105" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B105" s="63" t="s">
         <v>347</v>
       </c>
-      <c r="C104" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="D104" s="68"/>
-      <c r="E104" s="62"/>
-      <c r="F104" s="82"/>
-      <c r="G104" s="88">
+      <c r="C105" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D105" s="65"/>
+      <c r="E105" s="59"/>
+      <c r="F105" s="79"/>
+      <c r="G105" s="85">
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A105" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B105" s="57" t="s">
+    <row r="106" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A106" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B106" s="54" t="s">
         <v>331</v>
       </c>
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
-      <c r="E105" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="F105" s="57"/>
-      <c r="G105" s="6">
+      <c r="C106" s="54"/>
+      <c r="D106" s="54"/>
+      <c r="E106" s="54" t="s">
+        <v>282</v>
+      </c>
+      <c r="F106" s="54"/>
+      <c r="G106" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A106" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B106" s="25"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="F106" s="15"/>
-      <c r="G106" s="88">
+    <row r="107" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B107" s="25"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="F107" s="15"/>
+      <c r="G107" s="85">
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B107" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E107" s="7" t="s">
+    <row r="108" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B108" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D108" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="F107" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="G107" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A108" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B108" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="D108" s="93" t="s">
-        <v>378</v>
-      </c>
       <c r="E108" s="7" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="F108" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G108" s="88">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G108" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B109" s="37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>262</v>
+        <v>332</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>287</v>
+        <v>375</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="F109" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G109" s="6">
-        <v>20</v>
+      <c r="G109" s="85">
+        <v>19</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B110" s="37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F110" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G110" s="88">
-        <v>21</v>
+      <c r="G110" s="6">
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B111" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F111" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="G111" s="6">
+      <c r="G111" s="85">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B112" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="G112" s="6">
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B112" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="C112" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D112" s="26"/>
-      <c r="E112" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F112" s="30" t="s">
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B113" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C113" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" s="26"/>
+      <c r="E113" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F113" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="G112" s="88">
+      <c r="G113" s="85">
         <v>23</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B113" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C113" s="29" t="s">
-        <v>259</v>
-      </c>
-      <c r="D113" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="E113" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="F113" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="G113" s="6">
-        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>237</v>
+        <v>177</v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="G114" s="88">
-        <v>25</v>
+        <v>220</v>
+      </c>
+      <c r="G114" s="6">
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>348</v>
+        <v>296</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>301</v>
+        <v>239</v>
       </c>
       <c r="E115" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F115" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="G115" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="G115" s="85">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D116" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="E116" s="19" t="s">
         <v>303</v>
-      </c>
-      <c r="E116" s="19" t="s">
-        <v>304</v>
       </c>
       <c r="F116" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="G116" s="88">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G116" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B117" s="28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C117" s="29" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D117" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="E117" s="19" t="s">
         <v>305</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>306</v>
       </c>
       <c r="F117" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="G117" s="6">
+      <c r="G117" s="85">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C118" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="D118" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="E118" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="F118" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="G118" s="6">
         <v>28</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A118" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B118" s="66" t="s">
-        <v>317</v>
-      </c>
-      <c r="C118" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="D118" s="81"/>
-      <c r="E118" s="80"/>
-      <c r="F118" s="63"/>
-      <c r="G118" s="88">
+    <row r="119" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B119" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="C119" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="D119" s="78"/>
+      <c r="E119" s="77"/>
+      <c r="F119" s="60"/>
+      <c r="G119" s="85">
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="64" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A119" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B119" s="57" t="s">
+    <row r="120" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B120" s="54" t="s">
         <v>335</v>
       </c>
-      <c r="C119" s="57"/>
-      <c r="D119" s="57"/>
-      <c r="E119" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="F119" s="57"/>
-      <c r="G119" s="6">
+      <c r="C120" s="54"/>
+      <c r="D120" s="54"/>
+      <c r="E120" s="54" t="s">
+        <v>282</v>
+      </c>
+      <c r="F120" s="54"/>
+      <c r="G120" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A120" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B120" s="25"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="26"/>
-      <c r="E120" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="F120" s="15"/>
-      <c r="G120" s="88">
+    <row r="121" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A121" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B121" s="25"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="F121" s="15"/>
+      <c r="G121" s="85">
         <v>31</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A121" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B121" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="E121" s="7" t="s">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D122" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="F121" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G121" s="6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A122" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B122" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>253</v>
-      </c>
       <c r="E122" s="7" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="F122" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G122" s="88">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G122" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B123" s="10" t="s">
-        <v>98</v>
+        <v>234</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D123" s="7" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="E123" s="7" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="F123" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G123" s="6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="G123" s="85">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E124" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F124" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G124" s="88">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G124" s="6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B125" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="D125" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E125" s="7" t="s">
         <v>271</v>
-      </c>
-      <c r="E125" s="7" t="s">
-        <v>272</v>
       </c>
       <c r="F125" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G125" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="G125" s="85">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D126" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E126" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>274</v>
       </c>
       <c r="F126" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G126" s="88">
+      <c r="G126" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A127" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="G127" s="85">
         <v>37</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B127" s="59" t="s">
-        <v>318</v>
-      </c>
-      <c r="C127" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="D127" s="68"/>
-      <c r="E127" s="62"/>
-      <c r="F127" s="63"/>
-      <c r="G127" s="6">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B128" s="56" t="s">
+        <v>319</v>
+      </c>
+      <c r="C128" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D128" s="65"/>
+      <c r="E128" s="59"/>
+      <c r="F128" s="60"/>
+      <c r="G128" s="6">
         <v>38</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A128" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B128" s="48" t="s">
+    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A129" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B129" s="45" t="s">
         <v>356</v>
       </c>
-      <c r="C128" s="48"/>
-      <c r="D128" s="31"/>
-      <c r="E128" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="F128" s="15"/>
-      <c r="G128" s="88">
+      <c r="C129" s="45"/>
+      <c r="D129" s="31"/>
+      <c r="E129" s="54" t="s">
+        <v>282</v>
+      </c>
+      <c r="F129" s="15"/>
+      <c r="G129" s="85">
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="D129" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="E129" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F129" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G129" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C130" s="6" t="s">
         <v>323</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="F130" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G130" s="88">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G130" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B131" s="10" t="s">
-        <v>313</v>
+        <v>234</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="C131" s="6" t="s">
         <v>324</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="F131" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="G131" s="6">
+      <c r="G131" s="85">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>314</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E132" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F132" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="G132" s="6">
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A132" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B132" s="48"/>
-      <c r="C132" s="48"/>
-      <c r="D132" s="31"/>
-      <c r="E132" s="48" t="s">
+    <row r="133" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B133" s="45"/>
+      <c r="C133" s="45"/>
+      <c r="D133" s="31"/>
+      <c r="E133" s="45" t="s">
         <v>360</v>
       </c>
-      <c r="F132" s="15"/>
-      <c r="G132" s="88">
+      <c r="F133" s="15"/>
+      <c r="G133" s="85">
         <v>43</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="91" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A133" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B133" s="91" t="s">
+    <row r="134" spans="1:7" s="88" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B134" s="88" t="s">
         <v>362</v>
       </c>
-      <c r="C133" s="92" t="s">
-        <v>371</v>
-      </c>
-      <c r="D133" s="38" t="s">
+      <c r="C134" s="89" t="s">
+        <v>378</v>
+      </c>
+      <c r="D134" s="38" t="s">
         <v>361</v>
       </c>
-      <c r="E133" s="90" t="s">
+      <c r="E134" s="87" t="s">
         <v>365</v>
       </c>
-      <c r="F133" s="9"/>
-      <c r="G133" s="6">
+      <c r="F134" s="9"/>
+      <c r="G134" s="6">
         <v>44</v>
       </c>
     </row>
-    <row r="134" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B134" s="27" t="s">
+    <row r="135" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B135" s="27" t="s">
         <v>363</v>
       </c>
-      <c r="D134" s="9" t="s">
+      <c r="D135" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="G135" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B136" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E136" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="E134" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="G134" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A135" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B135" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="G135" s="88">
+      <c r="G136" s="85">
         <v>46</v>
       </c>
     </row>
-    <row r="136" spans="1:7" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="B136" s="25" t="s">
+    <row r="137" spans="1:7" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B137" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="C136" s="23"/>
-      <c r="D136" s="18"/>
-      <c r="E136" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="F136" s="15"/>
-      <c r="G136" s="6">
+      <c r="C137" s="23"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="F137" s="15"/>
+      <c r="G137" s="6">
         <v>47</v>
       </c>
     </row>
-    <row r="137" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="6"/>
-      <c r="B137" s="43"/>
-      <c r="C137" s="44"/>
-      <c r="D137" s="41"/>
-      <c r="E137" s="40"/>
-      <c r="G137" s="9"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B138" s="6"/>
-      <c r="D138" s="6"/>
-      <c r="E138" s="6"/>
-    </row>
-    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="6"/>
+      <c r="B138" s="41"/>
+      <c r="G138" s="9"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B139" s="6"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
     </row>
     <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B140" s="6"/>
-      <c r="C140" s="8"/>
       <c r="D140" s="6"/>
       <c r="E140" s="6"/>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B151" s="6"/>
-      <c r="D151" s="6"/>
-      <c r="E151" s="6"/>
+    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B141" s="6"/>
+      <c r="C141" s="8"/>
+      <c r="D141" s="6"/>
+      <c r="E141" s="6"/>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B152" s="6"/>
+      <c r="D152" s="6"/>
+      <c r="E152" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update hours of excursions
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Dropbox\Wood for Goods and Timber Conference\Programme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E55C7FA-1A24-4735-84D4-F2D33809F7AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F655176F-8959-494F-89DB-62D02E373874}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -1178,9 +1178,6 @@
     <t>(chair:  Jørgen Wadum)</t>
   </si>
   <si>
-    <t>15:15 - 19:00</t>
-  </si>
-  <si>
     <t>EXCURSIONS (boat trip on the Amsterdam canals, ...)</t>
   </si>
   <si>
@@ -1197,6 +1194,9 @@
   </si>
   <si>
     <t>Jan-Willem G. van de Kuilen</t>
+  </si>
+  <si>
+    <t>17:00 - 18:30</t>
   </si>
 </sst>
 </file>
@@ -1972,8 +1972,8 @@
   </sheetPr>
   <dimension ref="A1:I152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:A47"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2115,7 +2115,7 @@
         <v>327</v>
       </c>
       <c r="F8" s="52"/>
-      <c r="G8" s="6">
+      <c r="G8" s="53">
         <v>4</v>
       </c>
     </row>
@@ -2130,7 +2130,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="15"/>
-      <c r="G9" s="53">
+      <c r="G9" s="6">
         <v>5</v>
       </c>
     </row>
@@ -2153,7 +2153,7 @@
       <c r="F10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="53">
         <v>6</v>
       </c>
     </row>
@@ -2245,7 +2245,7 @@
       <c r="F14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="53">
         <v>10</v>
       </c>
       <c r="I14" s="11"/>
@@ -2265,7 +2265,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="30"/>
-      <c r="G15" s="53">
+      <c r="G15" s="6">
         <v>11</v>
       </c>
     </row>
@@ -2288,7 +2288,7 @@
       <c r="F16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="53">
         <v>12</v>
       </c>
     </row>
@@ -2380,7 +2380,7 @@
       <c r="F20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="53">
         <v>16</v>
       </c>
     </row>
@@ -2403,7 +2403,7 @@
       <c r="F21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="6">
         <v>17</v>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
       <c r="D22" s="58"/>
       <c r="E22" s="59"/>
       <c r="F22" s="60"/>
-      <c r="G22" s="6">
+      <c r="G22" s="53">
         <v>18</v>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       <c r="C24" s="35"/>
       <c r="D24" s="26"/>
       <c r="E24" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="53">
@@ -2499,7 +2499,7 @@
       <c r="F26" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="53">
         <v>22</v>
       </c>
     </row>
@@ -2522,7 +2522,7 @@
       <c r="F27" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="53">
+      <c r="G27" s="6">
         <v>23</v>
       </c>
     </row>
@@ -2545,7 +2545,7 @@
       <c r="F28" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="53">
         <v>24</v>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
         <v>91</v>
       </c>
       <c r="F32" s="15"/>
-      <c r="G32" s="6">
+      <c r="G32" s="53">
         <v>28</v>
       </c>
     </row>
@@ -2650,7 +2650,7 @@
       <c r="F33" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="G33" s="53">
+      <c r="G33" s="6">
         <v>29</v>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       <c r="F34" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="53">
         <v>30</v>
       </c>
     </row>
@@ -2765,7 +2765,7 @@
       <c r="F38" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="53">
         <v>34</v>
       </c>
     </row>
@@ -2784,7 +2784,7 @@
         <v>40</v>
       </c>
       <c r="F39" s="30"/>
-      <c r="G39" s="53">
+      <c r="G39" s="6">
         <v>35</v>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       <c r="F40" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="53">
         <v>36</v>
       </c>
     </row>
@@ -2899,7 +2899,7 @@
       <c r="F44" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="53">
         <v>40</v>
       </c>
     </row>
@@ -2916,7 +2916,7 @@
       <c r="D45" s="65"/>
       <c r="E45" s="59"/>
       <c r="F45" s="60"/>
-      <c r="G45" s="53">
+      <c r="G45" s="6">
         <v>41</v>
       </c>
     </row>
@@ -2933,7 +2933,7 @@
         <v>62</v>
       </c>
       <c r="F46" s="15"/>
-      <c r="G46" s="6">
+      <c r="G46" s="53">
         <v>42</v>
       </c>
     </row>
@@ -2971,7 +2971,7 @@
       <c r="F48" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="53">
+      <c r="G48" s="6">
         <v>44</v>
       </c>
     </row>
@@ -2994,7 +2994,7 @@
       <c r="F49" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49" s="53">
         <v>45</v>
       </c>
       <c r="I49" s="11"/>
@@ -3035,7 +3035,7 @@
         <v>345</v>
       </c>
       <c r="F51" s="13"/>
-      <c r="G51" s="53">
+      <c r="G51" s="6">
         <v>47</v>
       </c>
     </row>
@@ -3052,7 +3052,7 @@
         <v>140</v>
       </c>
       <c r="F52" s="13"/>
-      <c r="G52" s="6">
+      <c r="G52" s="53">
         <v>48</v>
       </c>
     </row>
@@ -3820,12 +3820,12 @@
         <v>142</v>
       </c>
       <c r="B89" s="82" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="C89" s="52"/>
       <c r="D89" s="52"/>
       <c r="E89" s="52" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F89" s="47"/>
       <c r="G89" s="85">
@@ -4064,7 +4064,7 @@
         <v>257</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E101" s="19" t="s">
         <v>258</v>
@@ -4228,7 +4228,7 @@
         <v>332</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>309</v>
@@ -4720,7 +4720,7 @@
         <v>314</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>276</v>
@@ -4758,7 +4758,7 @@
         <v>362</v>
       </c>
       <c r="C134" s="89" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D134" s="38" t="s">
         <v>361</v>

</xml_diff>

<commit_message>
update program with people not attending
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Dropbox\Wood for Goods and Timber Conference\Programme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F655176F-8959-494F-89DB-62D02E373874}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF7D990-C995-4E40-AF02-1505D6226375}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="374">
   <si>
     <t>day</t>
   </si>
@@ -390,12 +390,6 @@
     <t>S2-P-001</t>
   </si>
   <si>
-    <t>Abdelmoniem M. Abdelmoniem</t>
-  </si>
-  <si>
-    <t>Conservation processes of a painted wooden coffin at Saqqara area</t>
-  </si>
-  <si>
     <t>S2-P-002</t>
   </si>
   <si>
@@ -423,9 +417,6 @@
     <t>The Gribshunden Barrels</t>
   </si>
   <si>
-    <t>S2-P-005</t>
-  </si>
-  <si>
     <t>Ronald M. Visser</t>
   </si>
   <si>
@@ -576,12 +567,6 @@
     <t>S3-P-003</t>
   </si>
   <si>
-    <t>Rasha Shaheen</t>
-  </si>
-  <si>
-    <t>Preventive Conservation of Egyptian Wooden Statues back to Late Period Displayed at Egyptian Textile Museum</t>
-  </si>
-  <si>
     <t>S3-P-004</t>
   </si>
   <si>
@@ -589,9 +574,6 @@
   </si>
   <si>
     <t xml:space="preserve">Wooden artefacts from the castellum Velsen I, the Netherlands </t>
-  </si>
-  <si>
-    <t>S3-P-005</t>
   </si>
   <si>
     <t>Sytske Weidema</t>
@@ -692,9 +674,6 @@
     <t>12:30 - 12:45</t>
   </si>
   <si>
-    <t>S4-O-007</t>
-  </si>
-  <si>
     <t>Lisa Shindo</t>
   </si>
   <si>
@@ -1197,6 +1176,9 @@
   </si>
   <si>
     <t>17:00 - 18:30</t>
+  </si>
+  <si>
+    <t>S4-PR-001</t>
   </si>
 </sst>
 </file>
@@ -1970,10 +1952,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2059,7 +2041,7 @@
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="26" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="6">
@@ -2095,7 +2077,7 @@
         <v>108</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F7" s="52"/>
       <c r="G7" s="6">
@@ -2107,12 +2089,12 @@
         <v>11</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="54" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F8" s="52"/>
       <c r="G8" s="53">
@@ -2429,7 +2411,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
@@ -2449,7 +2431,7 @@
       <c r="C24" s="35"/>
       <c r="D24" s="26"/>
       <c r="E24" s="18" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="53">
@@ -2491,10 +2473,10 @@
         <v>70</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>68</v>
@@ -2581,7 +2563,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>113</v>
@@ -2619,7 +2601,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="26"/>
@@ -2631,7 +2613,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>11</v>
       </c>
@@ -2639,7 +2621,7 @@
         <v>92</v>
       </c>
       <c r="C33" s="83" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>94</v>
@@ -2648,13 +2630,13 @@
         <v>95</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="G33" s="6">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>11</v>
       </c>
@@ -2662,7 +2644,7 @@
         <v>96</v>
       </c>
       <c r="C34" s="83" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>101</v>
@@ -2671,13 +2653,13 @@
         <v>102</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="G34" s="53">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
         <v>11</v>
       </c>
@@ -2685,7 +2667,7 @@
         <v>100</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>97</v>
@@ -2700,7 +2682,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>11</v>
       </c>
@@ -2708,13 +2690,13 @@
         <v>103</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E36" s="66" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>99</v>
@@ -2723,7 +2705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>11</v>
       </c>
@@ -2731,7 +2713,7 @@
         <v>106</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>104</v>
@@ -2746,7 +2728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>11</v>
       </c>
@@ -2754,7 +2736,7 @@
         <v>111</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>108</v>
@@ -2769,7 +2751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
         <v>11</v>
       </c>
@@ -2788,7 +2770,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>11</v>
       </c>
@@ -2799,10 +2781,10 @@
         <v>117</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F40" s="14" t="s">
         <v>68</v>
@@ -2811,7 +2793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
         <v>11</v>
       </c>
@@ -2819,13 +2801,13 @@
         <v>41</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F41" s="14" t="s">
         <v>68</v>
@@ -2834,7 +2816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>11</v>
       </c>
@@ -2842,13 +2824,13 @@
         <v>41</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F42" s="14" t="s">
         <v>68</v>
@@ -2857,7 +2839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="9" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" s="9" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>11</v>
       </c>
@@ -2865,13 +2847,13 @@
         <v>41</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F43" s="14" t="s">
         <v>68</v>
@@ -2880,253 +2862,253 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="9" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="29" t="s">
+      <c r="B44" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>68</v>
-      </c>
+      <c r="C44" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44" s="65"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="60"/>
       <c r="G44" s="53">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="56" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="59"/>
-      <c r="F45" s="60"/>
+      <c r="B45" s="67" t="s">
+        <v>335</v>
+      </c>
+      <c r="C45" s="67"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="15"/>
       <c r="G45" s="6">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="67" t="s">
-        <v>342</v>
-      </c>
+      <c r="B46" s="67"/>
       <c r="C46" s="67"/>
       <c r="D46" s="23"/>
-      <c r="E46" s="54" t="s">
-        <v>62</v>
+      <c r="E46" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="F46" s="15"/>
       <c r="G46" s="53">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="67"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F47" s="15"/>
+      <c r="B47" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="G47" s="6">
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="F48" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48" s="53">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>137</v>
+        <v>307</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>135</v>
+        <v>66</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>136</v>
+        <v>67</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G49" s="53">
+      <c r="G49" s="6">
         <v>45</v>
       </c>
-      <c r="I49" s="11"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" s="6">
+      <c r="B50" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="C50" s="68"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="69" t="s">
+        <v>338</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="53">
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B51" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="C51" s="68"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="69" t="s">
-        <v>345</v>
+        <v>337</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="45" t="s">
+        <v>137</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="6">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="11" customFormat="1" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="48" t="s">
-        <v>344</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="45" t="s">
+    <row r="52" spans="1:9" s="9" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" s="71"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="74"/>
+    </row>
+    <row r="53" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="54" t="s">
+        <v>322</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="53">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="9" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="70" t="s">
+      <c r="F53" s="54"/>
+      <c r="G53" s="85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="25"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="C53" s="71"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="74"/>
-    </row>
-    <row r="54" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
+      <c r="F54" s="15"/>
+      <c r="G54" s="84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B54" s="54" t="s">
-        <v>329</v>
-      </c>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="54" t="s">
+      <c r="C55" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="F54" s="54"/>
-      <c r="G54" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="36" t="s">
+      <c r="D55" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="F55" s="15"/>
-      <c r="G55" s="84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="E55" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G55" s="85">
+        <v>3</v>
+      </c>
+      <c r="I55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F56" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G56" s="85">
-        <v>3</v>
-      </c>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G56" s="84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>150</v>
+        <v>13</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>151</v>
@@ -3138,18 +3120,19 @@
         <v>153</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G57" s="84">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G57" s="85">
+        <v>5</v>
+      </c>
+      <c r="I57" s="43"/>
+    </row>
+    <row r="58" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>154</v>
@@ -3161,19 +3144,18 @@
         <v>156</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G58" s="85">
-        <v>5</v>
-      </c>
-      <c r="I58" s="43"/>
-    </row>
-    <row r="59" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G58" s="84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>157</v>
@@ -3185,18 +3167,18 @@
         <v>159</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G59" s="84">
-        <v>6</v>
+        <v>146</v>
+      </c>
+      <c r="G59" s="85">
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>160</v>
@@ -3208,18 +3190,18 @@
         <v>162</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G60" s="85">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G60" s="84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>163</v>
@@ -3231,18 +3213,18 @@
         <v>165</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G61" s="84">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G61" s="85">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>166</v>
@@ -3254,57 +3236,57 @@
         <v>168</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G62" s="85">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G62" s="84">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="C63" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" s="30"/>
+      <c r="E63" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="30"/>
+      <c r="G63" s="85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="D64" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="F63" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="G63" s="84">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B64" s="25" t="s">
+      <c r="E64" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="C64" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D64" s="30"/>
-      <c r="E64" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F64" s="30"/>
-      <c r="G64" s="85">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F64" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G64" s="84">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B65" s="28" t="s">
         <v>41</v>
@@ -3319,15 +3301,15 @@
         <v>175</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G65" s="84">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G65" s="85">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B66" s="28" t="s">
         <v>41</v>
@@ -3336,166 +3318,166 @@
         <v>176</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G66" s="85">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="G66" s="84">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B67" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D67" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G67" s="85">
+        <v>15</v>
+      </c>
+      <c r="I67" s="75"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B68" s="63" t="s">
+        <v>182</v>
+      </c>
+      <c r="C68" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" s="64"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="60"/>
+      <c r="G68" s="84">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="54" t="s">
+        <v>323</v>
+      </c>
+      <c r="C69" s="54"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54" t="s">
         <v>183</v>
       </c>
-      <c r="E67" s="20" t="s">
+      <c r="F69" s="54"/>
+      <c r="G69" s="85">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" s="25"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="76" t="s">
         <v>184</v>
       </c>
-      <c r="F67" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G67" s="84">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="D68" s="20" t="s">
+      <c r="F70" s="47"/>
+      <c r="G70" s="84">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E71" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="F68" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G68" s="85">
-        <v>15</v>
-      </c>
-      <c r="I68" s="75"/>
-    </row>
-    <row r="69" spans="1:9" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B69" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C69" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="E69" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F69" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G69" s="84">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A70" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B70" s="63" t="s">
+      <c r="F71" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D70" s="64"/>
-      <c r="E70" s="59"/>
-      <c r="F70" s="60"/>
-      <c r="G70" s="85">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A71" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B71" s="54" t="s">
-        <v>330</v>
-      </c>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54" t="s">
+      <c r="G71" s="85">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="F71" s="54"/>
-      <c r="G71" s="85">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B72" s="25"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="76" t="s">
+      <c r="D72" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="F72" s="47"/>
+      <c r="E72" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>188</v>
+      </c>
       <c r="G72" s="84">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E73" s="4" t="s">
         <v>193</v>
       </c>
+      <c r="E73" s="5" t="s">
+        <v>194</v>
+      </c>
       <c r="F73" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G73" s="85">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>195</v>
@@ -3503,209 +3485,209 @@
       <c r="D74" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E74" s="5" t="s">
         <v>197</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G74" s="85">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="G74" s="84">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>198</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G75" s="84">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="G75" s="85">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>201</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G76" s="85">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="G76" s="84">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>81</v>
+        <v>204</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>204</v>
+        <v>373</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G77" s="84">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+      <c r="G77" s="85">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B78" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C78" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B78" s="63" t="s">
         <v>207</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="C78" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="D78" s="78"/>
+      <c r="E78" s="77"/>
+      <c r="F78" s="60"/>
+      <c r="G78" s="84">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A79" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" s="54" t="s">
+        <v>351</v>
+      </c>
+      <c r="C79" s="54"/>
+      <c r="D79" s="54"/>
+      <c r="E79" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G78" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A79" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B79" s="10" t="s">
+      <c r="F79" s="54"/>
+      <c r="G79" s="85">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" s="25"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="F80" s="15"/>
+      <c r="G80" s="84">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G81" s="85">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="C79" s="8" t="s">
+      <c r="D82" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="E82" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="F82" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F79" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G79" s="84">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="18" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" s="63" t="s">
+      <c r="G82" s="84">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A83" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="C80" s="77" t="s">
-        <v>90</v>
-      </c>
-      <c r="D80" s="78"/>
-      <c r="E80" s="77"/>
-      <c r="F80" s="60"/>
-      <c r="G80" s="85">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B81" s="54" t="s">
-        <v>358</v>
-      </c>
-      <c r="C81" s="54"/>
-      <c r="D81" s="54"/>
-      <c r="E81" s="54" t="s">
+      <c r="D83" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="F81" s="54"/>
-      <c r="G81" s="85">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B82" s="25"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="26"/>
-      <c r="E82" s="36" t="s">
-        <v>372</v>
-      </c>
-      <c r="F82" s="15"/>
-      <c r="G82" s="84">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A83" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>367</v>
-      </c>
       <c r="E83" s="7" t="s">
-        <v>368</v>
+        <v>216</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G83" s="85">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>217</v>
@@ -3717,1136 +3699,1090 @@
         <v>219</v>
       </c>
       <c r="F84" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G84" s="84">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A85" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C85" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="G84" s="84">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A85" s="9" t="s">
+      <c r="D85" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G85" s="85">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G86" s="84">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="24.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" s="82" t="s">
+        <v>372</v>
+      </c>
+      <c r="C87" s="52"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52" t="s">
+        <v>366</v>
+      </c>
+      <c r="F87" s="47"/>
+      <c r="G87" s="85">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="55" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="C88" s="72"/>
+      <c r="D88" s="80"/>
+      <c r="E88" s="81"/>
+      <c r="F88" s="74"/>
+    </row>
+    <row r="89" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A89" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B89" s="54" t="s">
+        <v>350</v>
+      </c>
+      <c r="C89" s="54"/>
+      <c r="D89" s="54"/>
+      <c r="E89" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="F89" s="54"/>
+      <c r="G89" s="85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B90" s="25"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="F90" s="30"/>
+      <c r="G90" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B91" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="B85" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G85" s="85">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A86" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G86" s="84">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A87" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="D87" s="7" t="s">
+      <c r="C91" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="E87" s="7" t="s">
+      <c r="D91" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="F87" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G87" s="85">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="C88" s="8" t="s">
+      <c r="E91" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G88" s="84">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="24.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B89" s="82" t="s">
-        <v>379</v>
-      </c>
-      <c r="C89" s="52"/>
-      <c r="D89" s="52"/>
-      <c r="E89" s="52" t="s">
-        <v>373</v>
-      </c>
-      <c r="F89" s="47"/>
-      <c r="G89" s="85">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="55" customFormat="1" ht="55.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="70" t="s">
-        <v>233</v>
-      </c>
-      <c r="C90" s="72"/>
-      <c r="D90" s="80"/>
-      <c r="E90" s="81"/>
-      <c r="F90" s="74"/>
-    </row>
-    <row r="91" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A91" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B91" s="54" t="s">
-        <v>357</v>
-      </c>
-      <c r="C91" s="54"/>
-      <c r="D91" s="54"/>
-      <c r="E91" s="54" t="s">
-        <v>215</v>
-      </c>
-      <c r="F91" s="54"/>
+      <c r="F91" s="9" t="s">
+        <v>213</v>
+      </c>
       <c r="G91" s="85">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G92" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="B92" s="25"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="F92" s="30"/>
-      <c r="G92" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A93" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="C93" s="8" t="s">
+      <c r="D93" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="E93" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="E93" s="7" t="s">
+      <c r="F93" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G93" s="85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="F93" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G93" s="85">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B94" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C94" s="8" t="s">
+      <c r="D94" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="E94" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="E94" s="7" t="s">
-        <v>240</v>
-      </c>
       <c r="F94" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G94" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C95" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D95" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="E95" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="E95" s="7" t="s">
+      <c r="F95" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G95" s="85">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="F95" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G95" s="85">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C96" s="8" t="s">
+      <c r="D96" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="E96" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="E96" s="7" t="s">
-        <v>246</v>
-      </c>
       <c r="F96" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G96" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>247</v>
+        <v>362</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G97" s="85">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B98" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C98" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B98" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="C98" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D98" s="26"/>
+      <c r="E98" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F98" s="30"/>
+      <c r="G98" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B99" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C99" s="33" t="s">
         <v>250</v>
       </c>
-      <c r="D98" s="7" t="s">
+      <c r="D99" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="E99" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="E98" s="7" t="s">
+      <c r="F99" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="G99" s="85">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B100" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100" s="33" t="s">
         <v>252</v>
       </c>
-      <c r="F98" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G98" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A99" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G99" s="85">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B100" s="25" t="s">
-        <v>346</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D100" s="26"/>
-      <c r="E100" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F100" s="30"/>
+      <c r="D100" s="19" t="s">
+        <v>352</v>
+      </c>
+      <c r="E100" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="G100" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C101" s="33" t="s">
-        <v>257</v>
+      <c r="C101" s="29" t="s">
+        <v>292</v>
       </c>
       <c r="D101" s="19" t="s">
-        <v>378</v>
+        <v>290</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>258</v>
+        <v>291</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>194</v>
+        <v>327</v>
       </c>
       <c r="G101" s="85">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="D102" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="E102" s="19" t="s">
-        <v>322</v>
+      <c r="C102" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D102" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="E102" s="20" t="s">
+        <v>274</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>194</v>
+        <v>327</v>
       </c>
       <c r="G102" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B103" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C103" s="29" t="s">
-        <v>299</v>
-      </c>
-      <c r="D103" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="E103" s="19" t="s">
-        <v>298</v>
-      </c>
-      <c r="F103" s="14" t="s">
-        <v>334</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B103" s="63" t="s">
+        <v>340</v>
+      </c>
+      <c r="C103" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D103" s="65"/>
+      <c r="E103" s="59"/>
+      <c r="F103" s="79"/>
       <c r="G103" s="85">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B104" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C104" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="D104" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E104" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="F104" s="14" t="s">
-        <v>334</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B104" s="54" t="s">
+        <v>324</v>
+      </c>
+      <c r="C104" s="54"/>
+      <c r="D104" s="54"/>
+      <c r="E104" s="54" t="s">
+        <v>275</v>
+      </c>
+      <c r="F104" s="54"/>
       <c r="G104" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B105" s="63" t="s">
-        <v>347</v>
-      </c>
-      <c r="C105" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D105" s="65"/>
-      <c r="E105" s="59"/>
-      <c r="F105" s="79"/>
+        <v>227</v>
+      </c>
+      <c r="B105" s="25"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="F105" s="15"/>
       <c r="G105" s="85">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B106" s="54" t="s">
-        <v>331</v>
-      </c>
-      <c r="C106" s="54"/>
-      <c r="D106" s="54"/>
-      <c r="E106" s="54" t="s">
-        <v>282</v>
-      </c>
-      <c r="F106" s="54"/>
+        <v>227</v>
+      </c>
+      <c r="B106" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>326</v>
+      </c>
       <c r="G106" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B107" s="25"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="36" t="s">
-        <v>283</v>
-      </c>
-      <c r="F107" s="15"/>
+        <v>227</v>
+      </c>
+      <c r="B107" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>326</v>
+      </c>
       <c r="G107" s="85">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B108" s="37" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="D108" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="G108" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A109" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B109" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E109" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E108" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="G108" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A109" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B109" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="D109" s="7" t="s">
-        <v>374</v>
-      </c>
-      <c r="E109" s="7" t="s">
-        <v>309</v>
-      </c>
       <c r="F109" s="9" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G109" s="85">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B110" s="37" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D110" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E110" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="E110" s="7" t="s">
+      <c r="F110" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="G110" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B111" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="C111" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="26"/>
+      <c r="E111" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F111" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="G111" s="85">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B112" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C112" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="F112" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="G112" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C113" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="F110" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="G110" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A111" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B111" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E111" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="G111" s="85">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A112" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B112" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="G112" s="6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B113" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="C113" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D113" s="26"/>
-      <c r="E113" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F113" s="30" t="s">
-        <v>336</v>
+      <c r="D113" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="E113" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F113" s="14" t="s">
+        <v>326</v>
       </c>
       <c r="G113" s="85">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B114" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>260</v>
+        <v>341</v>
       </c>
       <c r="D114" s="19" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
       <c r="E114" s="19" t="s">
-        <v>261</v>
+        <v>296</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>220</v>
+        <v>326</v>
       </c>
       <c r="G114" s="6">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B115" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>296</v>
+        <v>342</v>
       </c>
       <c r="D115" s="19" t="s">
-        <v>239</v>
+        <v>297</v>
       </c>
       <c r="E115" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G115" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B116" s="28" t="s">
         <v>41</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D116" s="19" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E116" s="19" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="G116" s="6">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B117" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C117" s="29" t="s">
-        <v>349</v>
-      </c>
-      <c r="D117" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="F117" s="14" t="s">
-        <v>333</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B117" s="63" t="s">
+        <v>311</v>
+      </c>
+      <c r="C117" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="D117" s="78"/>
+      <c r="E117" s="77"/>
+      <c r="F117" s="60"/>
       <c r="G117" s="85">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B118" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C118" s="29" t="s">
-        <v>350</v>
-      </c>
-      <c r="D118" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="E118" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="F118" s="14" t="s">
-        <v>333</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B118" s="54" t="s">
+        <v>328</v>
+      </c>
+      <c r="C118" s="54"/>
+      <c r="D118" s="54"/>
+      <c r="E118" s="54" t="s">
+        <v>275</v>
+      </c>
+      <c r="F118" s="54"/>
       <c r="G118" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B119" s="63" t="s">
-        <v>318</v>
-      </c>
-      <c r="C119" s="77" t="s">
-        <v>90</v>
-      </c>
-      <c r="D119" s="78"/>
-      <c r="E119" s="77"/>
-      <c r="F119" s="60"/>
+        <v>227</v>
+      </c>
+      <c r="B119" s="25"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="F119" s="15"/>
       <c r="G119" s="85">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" s="61" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B120" s="54" t="s">
-        <v>335</v>
-      </c>
-      <c r="C120" s="54"/>
-      <c r="D120" s="54"/>
-      <c r="E120" s="54" t="s">
-        <v>282</v>
-      </c>
-      <c r="F120" s="54"/>
+        <v>227</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>327</v>
+      </c>
       <c r="G120" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B121" s="25"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="26"/>
-      <c r="E121" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="F121" s="15"/>
+        <v>227</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>327</v>
+      </c>
       <c r="G121" s="85">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D122" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G122" s="6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E123" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="E122" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="F122" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G122" s="6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A123" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>256</v>
-      </c>
       <c r="F123" s="9" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G123" s="85">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="D124" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F124" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G124" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D125" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="E124" s="7" t="s">
+      <c r="E125" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="F124" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G124" s="6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A125" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B125" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="E125" s="7" t="s">
-        <v>271</v>
-      </c>
       <c r="F125" s="9" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G125" s="85">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B126" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D126" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E126" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="F126" s="9" t="s">
-        <v>334</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B126" s="56" t="s">
+        <v>312</v>
+      </c>
+      <c r="C126" s="64" t="s">
+        <v>61</v>
+      </c>
+      <c r="D126" s="65"/>
+      <c r="E126" s="59"/>
+      <c r="F126" s="60"/>
       <c r="G126" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B127" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="E127" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B127" s="45" t="s">
+        <v>349</v>
+      </c>
+      <c r="C127" s="45"/>
+      <c r="D127" s="31"/>
+      <c r="E127" s="54" t="s">
         <v>275</v>
       </c>
-      <c r="F127" s="9" t="s">
-        <v>334</v>
-      </c>
+      <c r="F127" s="15"/>
       <c r="G127" s="85">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B128" s="56" t="s">
-        <v>319</v>
-      </c>
-      <c r="C128" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="D128" s="65"/>
-      <c r="E128" s="59"/>
-      <c r="F128" s="60"/>
+        <v>227</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>327</v>
+      </c>
       <c r="G128" s="6">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B129" s="45" t="s">
-        <v>356</v>
-      </c>
-      <c r="C129" s="45"/>
-      <c r="D129" s="31"/>
-      <c r="E129" s="54" t="s">
-        <v>282</v>
-      </c>
-      <c r="F129" s="15"/>
+        <v>227</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="F129" s="9" t="s">
+        <v>327</v>
+      </c>
       <c r="G129" s="85">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>133</v>
+        <v>227</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>307</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>323</v>
+        <v>369</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G130" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B131" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="E131" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="F131" s="9" t="s">
-        <v>334</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B131" s="45"/>
+      <c r="C131" s="45"/>
+      <c r="D131" s="31"/>
+      <c r="E131" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="F131" s="15"/>
       <c r="G131" s="85">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" s="88" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B132" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B132" s="88" t="s">
+        <v>355</v>
+      </c>
+      <c r="C132" s="89" t="s">
+        <v>370</v>
+      </c>
+      <c r="D132" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="E132" s="87" t="s">
+        <v>358</v>
+      </c>
+      <c r="F132" s="9"/>
+      <c r="G132" s="6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B133" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="D133" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="C132" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="D132" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="E132" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="F132" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="G132" s="6">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A133" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B133" s="45"/>
-      <c r="C133" s="45"/>
-      <c r="D133" s="31"/>
-      <c r="E133" s="45" t="s">
-        <v>360</v>
-      </c>
-      <c r="F133" s="15"/>
-      <c r="G133" s="85">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" s="88" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="E133" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="G133" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B134" s="88" t="s">
-        <v>362</v>
-      </c>
-      <c r="C134" s="89" t="s">
-        <v>377</v>
-      </c>
-      <c r="D134" s="38" t="s">
-        <v>361</v>
-      </c>
-      <c r="E134" s="87" t="s">
-        <v>365</v>
-      </c>
-      <c r="F134" s="9"/>
-      <c r="G134" s="6">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+      <c r="B134" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="D134" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E134" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G134" s="85">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B135" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>364</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="B135" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="C135" s="23"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F135" s="15"/>
       <c r="G135" s="6">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A136" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B136" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="D136" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E136" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="G136" s="85">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B137" s="25" t="s">
-        <v>354</v>
-      </c>
-      <c r="C137" s="23"/>
-      <c r="D137" s="18"/>
-      <c r="E137" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="F137" s="15"/>
-      <c r="G137" s="6">
         <v>47</v>
       </c>
     </row>
-    <row r="138" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="6"/>
-      <c r="B138" s="41"/>
-      <c r="G138" s="9"/>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6"/>
+      <c r="B136" s="41"/>
+      <c r="G136" s="9"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B137" s="6"/>
+      <c r="D137" s="6"/>
+      <c r="E137" s="6"/>
+    </row>
+    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B138" s="6"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="6"/>
+    </row>
+    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="6"/>
+      <c r="C139" s="8"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
     </row>
-    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="6"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="6"/>
-    </row>
-    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="6"/>
-      <c r="C141" s="8"/>
-      <c r="D141" s="6"/>
-      <c r="E141" s="6"/>
-    </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B152" s="6"/>
-      <c r="D152" s="6"/>
-      <c r="E152" s="6"/>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B150" s="6"/>
+      <c r="D150" s="6"/>
+      <c r="E150" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
previous commit failed to update website
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF7D990-C995-4E40-AF02-1505D6226375}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBC1640-5C6A-4DEC-BA01-19D6CBA95E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -977,9 +977,6 @@
     <t>Old Wood in a New Light – A dendrochronological database</t>
   </si>
   <si>
-    <t>DINNER &amp; PARTY</t>
-  </si>
-  <si>
     <t>16:00 - 16:15</t>
   </si>
   <si>
@@ -1157,9 +1154,6 @@
     <t>(chair:  Jørgen Wadum)</t>
   </si>
   <si>
-    <t>EXCURSIONS (boat trip on the Amsterdam canals, ...)</t>
-  </si>
-  <si>
     <t>Manu Frederickx</t>
   </si>
   <si>
@@ -1179,6 +1173,12 @@
   </si>
   <si>
     <t>S4-PR-001</t>
+  </si>
+  <si>
+    <t>EXCURSIONS (boat trip on the Amsterdam canals, with drinks and snacks)</t>
+  </si>
+  <si>
+    <t>DINNER &amp; PARTY at Restaurant 'De Kroon'</t>
   </si>
 </sst>
 </file>
@@ -1954,8 +1954,8 @@
   </sheetPr>
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2041,7 +2041,7 @@
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="6">
@@ -2077,7 +2077,7 @@
         <v>108</v>
       </c>
       <c r="E7" s="51" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F7" s="52"/>
       <c r="G7" s="6">
@@ -2089,12 +2089,12 @@
         <v>11</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F8" s="52"/>
       <c r="G8" s="53">
@@ -2411,7 +2411,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C23" s="54"/>
       <c r="D23" s="54"/>
@@ -2431,7 +2431,7 @@
       <c r="C24" s="35"/>
       <c r="D24" s="26"/>
       <c r="E24" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="53">
@@ -2563,7 +2563,7 @@
         <v>85</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>113</v>
@@ -2601,7 +2601,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="45" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="26"/>
@@ -2621,7 +2621,7 @@
         <v>92</v>
       </c>
       <c r="C33" s="83" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D33" s="38" t="s">
         <v>94</v>
@@ -2630,7 +2630,7 @@
         <v>95</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G33" s="6">
         <v>29</v>
@@ -2644,7 +2644,7 @@
         <v>96</v>
       </c>
       <c r="C34" s="83" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>101</v>
@@ -2653,7 +2653,7 @@
         <v>102</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G34" s="53">
         <v>30</v>
@@ -2667,7 +2667,7 @@
         <v>100</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>97</v>
@@ -2690,13 +2690,13 @@
         <v>103</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E36" s="66" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>99</v>
@@ -2713,7 +2713,7 @@
         <v>106</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D37" s="38" t="s">
         <v>104</v>
@@ -2736,7 +2736,7 @@
         <v>111</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>108</v>
@@ -2884,7 +2884,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="67" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C45" s="67"/>
       <c r="D45" s="23"/>
@@ -2963,7 +2963,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>131</v>
@@ -2986,12 +2986,12 @@
         <v>11</v>
       </c>
       <c r="B50" s="48" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C50" s="68"/>
       <c r="D50" s="32"/>
       <c r="E50" s="69" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F50" s="13"/>
       <c r="G50" s="53">
@@ -3003,7 +3003,7 @@
         <v>11</v>
       </c>
       <c r="B51" s="48" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -3029,7 +3029,7 @@
         <v>139</v>
       </c>
       <c r="B53" s="54" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="54"/>
@@ -3376,7 +3376,7 @@
         <v>139</v>
       </c>
       <c r="B69" s="54" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C69" s="54"/>
       <c r="D69" s="54"/>
@@ -3549,7 +3549,7 @@
         <v>204</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>199</v>
@@ -3586,7 +3586,7 @@
         <v>139</v>
       </c>
       <c r="B79" s="54" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C79" s="54"/>
       <c r="D79" s="54"/>
@@ -3606,7 +3606,7 @@
       <c r="C80" s="26"/>
       <c r="D80" s="26"/>
       <c r="E80" s="36" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F80" s="15"/>
       <c r="G80" s="84">
@@ -3624,10 +3624,10 @@
         <v>107</v>
       </c>
       <c r="D81" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="E81" s="7" t="s">
         <v>360</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>361</v>
       </c>
       <c r="F81" s="9" t="s">
         <v>213</v>
@@ -3733,7 +3733,7 @@
         <v>139</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>223</v>
@@ -3756,12 +3756,12 @@
         <v>139</v>
       </c>
       <c r="B87" s="82" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C87" s="52"/>
       <c r="D87" s="52"/>
       <c r="E87" s="52" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="F87" s="47"/>
       <c r="G87" s="85">
@@ -3782,7 +3782,7 @@
         <v>227</v>
       </c>
       <c r="B89" s="54" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C89" s="54"/>
       <c r="D89" s="54"/>
@@ -3955,7 +3955,7 @@
         <v>30</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>224</v>
@@ -3975,7 +3975,7 @@
         <v>227</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C98" s="34" t="s">
         <v>39</v>
@@ -4000,7 +4000,7 @@
         <v>250</v>
       </c>
       <c r="D99" s="19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E99" s="19" t="s">
         <v>251</v>
@@ -4023,10 +4023,10 @@
         <v>252</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F100" s="14" t="s">
         <v>188</v>
@@ -4052,7 +4052,7 @@
         <v>291</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G101" s="85">
         <v>13</v>
@@ -4075,7 +4075,7 @@
         <v>274</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G102" s="6">
         <v>14</v>
@@ -4086,7 +4086,7 @@
         <v>227</v>
       </c>
       <c r="B103" s="63" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C103" s="64" t="s">
         <v>61</v>
@@ -4103,7 +4103,7 @@
         <v>227</v>
       </c>
       <c r="B104" s="54" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C104" s="54"/>
       <c r="D104" s="54"/>
@@ -4147,7 +4147,7 @@
         <v>279</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G106" s="6">
         <v>18</v>
@@ -4161,22 +4161,22 @@
         <v>69</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>302</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G107" s="85">
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" s="9" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>227</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>282</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G108" s="6">
         <v>20</v>
@@ -4216,7 +4216,7 @@
         <v>285</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G109" s="85">
         <v>21</v>
@@ -4239,7 +4239,7 @@
         <v>288</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G110" s="6">
         <v>22</v>
@@ -4250,7 +4250,7 @@
         <v>227</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C111" s="34" t="s">
         <v>39</v>
@@ -4260,7 +4260,7 @@
         <v>40</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G111" s="85">
         <v>23</v>
@@ -4306,7 +4306,7 @@
         <v>293</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G113" s="85">
         <v>25</v>
@@ -4320,7 +4320,7 @@
         <v>41</v>
       </c>
       <c r="C114" s="29" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D114" s="19" t="s">
         <v>295</v>
@@ -4329,7 +4329,7 @@
         <v>296</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G114" s="6">
         <v>26</v>
@@ -4343,7 +4343,7 @@
         <v>41</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D115" s="19" t="s">
         <v>297</v>
@@ -4352,7 +4352,7 @@
         <v>298</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G115" s="85">
         <v>27</v>
@@ -4366,7 +4366,7 @@
         <v>41</v>
       </c>
       <c r="C116" s="29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D116" s="19" t="s">
         <v>299</v>
@@ -4375,7 +4375,7 @@
         <v>300</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G116" s="6">
         <v>28</v>
@@ -4386,7 +4386,7 @@
         <v>227</v>
       </c>
       <c r="B117" s="63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C117" s="77" t="s">
         <v>90</v>
@@ -4403,7 +4403,7 @@
         <v>227</v>
       </c>
       <c r="B118" s="54" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C118" s="54"/>
       <c r="D118" s="54"/>
@@ -4447,7 +4447,7 @@
         <v>258</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G120" s="6">
         <v>32</v>
@@ -4470,7 +4470,7 @@
         <v>249</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G121" s="85">
         <v>33</v>
@@ -4493,7 +4493,7 @@
         <v>261</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G122" s="6">
         <v>34</v>
@@ -4516,7 +4516,7 @@
         <v>264</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G123" s="85">
         <v>35</v>
@@ -4539,7 +4539,7 @@
         <v>266</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G124" s="6">
         <v>36</v>
@@ -4562,7 +4562,7 @@
         <v>268</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G125" s="85">
         <v>37</v>
@@ -4573,7 +4573,7 @@
         <v>227</v>
       </c>
       <c r="B126" s="56" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C126" s="64" t="s">
         <v>61</v>
@@ -4590,7 +4590,7 @@
         <v>227</v>
       </c>
       <c r="B127" s="45" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C127" s="45"/>
       <c r="D127" s="31"/>
@@ -4610,7 +4610,7 @@
         <v>130</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>271</v>
@@ -4619,7 +4619,7 @@
         <v>272</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G128" s="6">
         <v>40</v>
@@ -4633,7 +4633,7 @@
         <v>134</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>304</v>
@@ -4642,7 +4642,7 @@
         <v>305</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G129" s="85">
         <v>41</v>
@@ -4653,10 +4653,10 @@
         <v>227</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>269</v>
@@ -4665,7 +4665,7 @@
         <v>270</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G130" s="6">
         <v>42</v>
@@ -4679,7 +4679,7 @@
       <c r="C131" s="45"/>
       <c r="D131" s="31"/>
       <c r="E131" s="45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F131" s="15"/>
       <c r="G131" s="85">
@@ -4691,16 +4691,16 @@
         <v>227</v>
       </c>
       <c r="B132" s="88" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C132" s="89" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D132" s="38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E132" s="87" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F132" s="9"/>
       <c r="G132" s="6">
@@ -4712,13 +4712,13 @@
         <v>227</v>
       </c>
       <c r="B133" s="27" t="s">
+        <v>355</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E133" s="9" t="s">
         <v>356</v>
-      </c>
-      <c r="D133" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="E133" s="9" t="s">
-        <v>357</v>
       </c>
       <c r="G133" s="6">
         <v>45</v>
@@ -4729,13 +4729,13 @@
         <v>227</v>
       </c>
       <c r="B134" s="27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D134" s="9" t="s">
         <v>15</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G134" s="85">
         <v>46</v>
@@ -4746,12 +4746,12 @@
         <v>227</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C135" s="23"/>
       <c r="D135" s="18"/>
       <c r="E135" s="26" t="s">
-        <v>306</v>
+        <v>373</v>
       </c>
       <c r="F135" s="15"/>
       <c r="G135" s="6">

</xml_diff>

<commit_message>
fixed title error session 7
</commit_message>
<xml_diff>
--- a/ForHer22_PROGRAM.xlsx
+++ b/ForHer22_PROGRAM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanecakr\Documents\R_github\forests2heritage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9734B45-11C1-4875-B421-81CDDE63A222}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8628B9-E0C5-4D36-BE53-56B8C412DCA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="792" xr2:uid="{17DECA21-1FE6-4758-AA98-733CFD1E0FA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="377">
   <si>
     <t>day</t>
   </si>
@@ -1185,6 +1185,9 @@
   </si>
   <si>
     <t>Kickoff</t>
+  </si>
+  <si>
+    <t>Novel methods for dating and provenance analysis</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1963,8 @@
   </sheetPr>
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4431,7 +4434,7 @@
       <c r="C119" s="54"/>
       <c r="D119" s="54"/>
       <c r="E119" s="54" t="s">
-        <v>273</v>
+        <v>376</v>
       </c>
       <c r="F119" s="54"/>
       <c r="G119" s="6">
@@ -4618,7 +4621,7 @@
       <c r="C128" s="45"/>
       <c r="D128" s="31"/>
       <c r="E128" s="54" t="s">
-        <v>273</v>
+        <v>376</v>
       </c>
       <c r="F128" s="15"/>
       <c r="G128" s="85">

</xml_diff>